<commit_message>
fucking annoying timing adjustment....
</commit_message>
<xml_diff>
--- a/doc/mos6502-clock.xlsx
+++ b/doc/mos6502-clock.xlsx
@@ -558,16 +558,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>125</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>131</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -576,11 +576,15 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10201275" y="21440775"/>
+          <a:off x="9858375" y="23660100"/>
           <a:ext cx="1409700" cy="1038225"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
-          <a:avLst/>
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -7995"/>
+            <a:gd name="adj2" fmla="val -76950"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
         </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
@@ -1104,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:J156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="W137" sqref="W137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
yes, we finally found you bastard!
nmi handling had the bug!!
must be eliminated...
</commit_message>
<xml_diff>
--- a/doc/mos6502-clock.xlsx
+++ b/doc/mos6502-clock.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="28035" windowHeight="13920"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="28035" windowHeight="13920" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="clock" sheetId="1" r:id="rId1"/>
-    <sheet name="debug emu" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="logic analyzer nmi debug" sheetId="4" r:id="rId2"/>
+    <sheet name="debug emu" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
   <si>
     <t>---DE1 base clock 50 MHz</t>
   </si>
@@ -319,10 +320,48 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>拡大</t>
+    <t>DMA終了部</t>
+    <rPh sb="3" eb="5">
+      <t>シュウリョウ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ブ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>DMA 開始部</t>
+    <rPh sb="4" eb="6">
+      <t>カイシ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ブ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>正常パターン</t>
     <rPh sb="0" eb="2">
-      <t>カクダイ</t>
+      <t>セイジョウ</t>
     </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>異常パターン</t>
+    <rPh sb="0" eb="2">
+      <t>イジョウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>&lt;&lt;RTIのstackが破壊されてる</t>
+    <rPh sb="12" eb="14">
+      <t>ハカイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>normally like this…</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -330,7 +369,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,6 +388,22 @@
     </font>
     <font>
       <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
@@ -380,7 +435,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -402,6 +457,12 @@
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="桁区切り" xfId="1" builtinId="6"/>
@@ -418,24 +479,71 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>167</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>89</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>213</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 10"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1371600" y="35509200"/>
+          <a:ext cx="15316200" cy="7991475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -465,24 +573,24 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>108</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>149</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPr id="4" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -490,7 +598,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1371600" y="18859500"/>
+          <a:off x="1371600" y="18516600"/>
           <a:ext cx="14458950" cy="7124700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -512,18 +620,18 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>131</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>136</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="角丸四角形 3"/>
+        <xdr:cNvPr id="5" name="角丸四角形 4"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -567,18 +675,18 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>138</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>144</xdr:row>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="角丸四角形吹き出し 4"/>
+        <xdr:cNvPr id="6" name="角丸四角形吹き出し 5"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -626,24 +734,24 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>157</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>533401</xdr:colOff>
-      <xdr:row>184</xdr:row>
+      <xdr:row>146</xdr:row>
       <xdr:rowOff>23026</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1027" name="Picture 3"/>
+        <xdr:cNvPr id="7" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -673,24 +781,24 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>156</xdr:row>
+      <xdr:row>118</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>184</xdr:row>
+      <xdr:row>146</xdr:row>
       <xdr:rowOff>14959</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1028" name="Picture 4"/>
+        <xdr:cNvPr id="8" name="Picture 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -720,18 +828,18 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>164</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>170</xdr:row>
+      <xdr:row>132</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="角丸四角形吹き出し 7"/>
+        <xdr:cNvPr id="9" name="角丸四角形吹き出し 8"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -775,18 +883,18 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>174</xdr:row>
+      <xdr:row>136</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>180</xdr:row>
+      <xdr:row>142</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="右矢印 8"/>
+        <xdr:cNvPr id="10" name="右矢印 9"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -829,24 +937,24 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>192</xdr:row>
+      <xdr:row>373</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>238</xdr:row>
+      <xdr:row>419</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="11" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -854,7 +962,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1371600" y="32918400"/>
+          <a:off x="1371600" y="71189850"/>
           <a:ext cx="15316200" cy="7991475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -876,24 +984,24 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>240</xdr:row>
+      <xdr:row>421</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>286</xdr:row>
+      <xdr:row>467</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="12" name="Picture 5"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -901,7 +1009,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1371600" y="41148000"/>
+          <a:off x="1371600" y="79419450"/>
           <a:ext cx="15316200" cy="7991475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -917,6 +1025,984 @@
         <a:effectLst/>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>472</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>518</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1371600" y="88163400"/>
+          <a:ext cx="15316200" cy="7991475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>520</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>566</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1371600" y="96393000"/>
+          <a:ext cx="15316200" cy="7991475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>270</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>316</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1371600" y="53168550"/>
+          <a:ext cx="15316200" cy="7991475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>319</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>365</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1371600" y="61569600"/>
+          <a:ext cx="15316200" cy="7991475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>194</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>200</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="角丸四角形吹き出し 16"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7896225" y="40195500"/>
+          <a:ext cx="1666875" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 52311"/>
+            <a:gd name="adj2" fmla="val -196154"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>next instruction</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>837b</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>297</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>303</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="角丸四角形吹き出し 17"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4914900" y="57959625"/>
+          <a:ext cx="1666875" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 28882"/>
+            <a:gd name="adj2" fmla="val -188461"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>next instruction</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>402</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>408</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="角丸四角形吹き出し 18"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4781550" y="76314300"/>
+          <a:ext cx="1666875" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 106025"/>
+            <a:gd name="adj2" fmla="val -154808"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>next instruction</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>837b</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:row>498</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>504</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="角丸四角形吹き出し 19"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4514850" y="92697300"/>
+          <a:ext cx="1666875" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 66025"/>
+            <a:gd name="adj2" fmla="val -179808"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>next instruction</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>215</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>261</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1371600" y="43738800"/>
+          <a:ext cx="15316200" cy="7991475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>298</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>304</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="角丸四角形吹き出し 21"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10363200" y="58045350"/>
+          <a:ext cx="1666875" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 28882"/>
+            <a:gd name="adj2" fmla="val -188461"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>RTI return addr 8099</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>288</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>290</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="角丸四角形 22"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11220450" y="56254650"/>
+          <a:ext cx="1200150" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>500</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>506</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="角丸四角形吹き出し 23"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10487025" y="93049725"/>
+          <a:ext cx="1666875" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 28882"/>
+            <a:gd name="adj2" fmla="val -188461"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>RTI return addr </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>994C</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Someboy broke addr 01fe with 4C!!!</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>490</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>492</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="角丸四角形 24"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11344275" y="91259025"/>
+          <a:ext cx="1200150" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>575</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>621</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1371600" y="105822750"/>
+          <a:ext cx="15316200" cy="7991475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>602</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>608</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="角丸四角形吹き出し 26"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10153650" y="110594775"/>
+          <a:ext cx="1666875" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 28882"/>
+            <a:gd name="adj2" fmla="val -188461"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>This guy just broke the memory!!</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>626</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>672</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1371600" y="114566700"/>
+          <a:ext cx="15316200" cy="7991475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>653</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>659</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="角丸四角形吹き出し 28"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10496550" y="119338725"/>
+          <a:ext cx="1666875" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 28882"/>
+            <a:gd name="adj2" fmla="val -188461"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>return</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> to 8099</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1207,10 +2293,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:J192"/>
+  <dimension ref="A3:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="S189" sqref="S189"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1433,7 +2519,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="2:9">
+    <row r="33" spans="2:5">
       <c r="C33" s="6">
         <f>C29+$C$24</f>
         <v>67747</v>
@@ -1446,7 +2532,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="2:5">
       <c r="C34" t="str">
         <f>DEC2HEX(C33)</f>
         <v>108A3</v>
@@ -1455,12 +2541,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:5">
       <c r="B36" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="2:9">
+    <row r="37" spans="2:5">
       <c r="C37" s="6">
         <f>C33+$C$24</f>
         <v>102747</v>
@@ -1470,7 +2556,7 @@
         <v>49318560</v>
       </c>
     </row>
-    <row r="38" spans="2:9">
+    <row r="38" spans="2:5">
       <c r="C38" t="str">
         <f>DEC2HEX(C37)</f>
         <v>1915B</v>
@@ -1479,136 +2565,251 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="2:5">
       <c r="B40" t="str">
         <f>E40&amp;"回目のvblankは"</f>
-        <v>9回目のvblankは</v>
+        <v>8回目のvblankは</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>29</v>
       </c>
       <c r="E40" s="3">
-        <v>9</v>
-      </c>
-      <c r="G40" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5">
       <c r="C41" s="6">
         <f>$C$29+$C$24*(E40-1)</f>
-        <v>312747</v>
+        <v>277747</v>
       </c>
       <c r="D41" s="1">
         <f>C41*$D$13</f>
-        <v>150118560</v>
-      </c>
-      <c r="G41" t="s">
-        <v>36</v>
-      </c>
-      <c r="I41" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9">
+        <v>133318560</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5">
       <c r="C42" t="str">
         <f>DEC2HEX(C41)</f>
-        <v>4C5AB</v>
+        <v>43CF3</v>
       </c>
       <c r="D42" t="s">
         <v>26</v>
-      </c>
-      <c r="G42">
-        <v>10</v>
-      </c>
-      <c r="I42" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1">
-      <c r="A94" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1">
-      <c r="A95" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1">
-      <c r="A96" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1">
-      <c r="A97" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1">
-      <c r="A99" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1">
-      <c r="A102" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1">
-      <c r="A103" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1">
-      <c r="A104" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1">
-      <c r="A106" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1">
-      <c r="A107" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="154" spans="3:3">
-      <c r="C154" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="155" spans="3:3">
-      <c r="C155" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="156" spans="3:3">
-      <c r="C156" t="str">
-        <f>DEC2HEX(HEX2DEC(C155)-35000)</f>
-        <v>44626</v>
-      </c>
-    </row>
-    <row r="192" spans="3:3">
-      <c r="C192" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:E626"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="12.125" customWidth="1"/>
+    <col min="5" max="5" width="16.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="116" spans="3:3">
+      <c r="C116" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="117" spans="3:3">
+      <c r="C117" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="118" spans="3:3">
+      <c r="C118" t="str">
+        <f>DEC2HEX(HEX2DEC(C117)-35000)</f>
+        <v>44626</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="A159" t="s">
+        <v>59</v>
+      </c>
+      <c r="E159" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="A160" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="42">
+      <c r="C166" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="C167" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="270" spans="3:3">
+      <c r="C270" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="372" spans="3:3" ht="42">
+      <c r="C372" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="373" spans="3:3">
+      <c r="C373" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="472" spans="3:3">
+      <c r="C472" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="626" spans="3:3">
+      <c r="C626" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:B26"/>
   <sheetViews>
@@ -1717,7 +2918,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
nmi, jmp rti bug investigation...
</commit_message>
<xml_diff>
--- a/doc/mos6502-clock.xlsx
+++ b/doc/mos6502-clock.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="76">
   <si>
     <t>---DE1 base clock 50 MHz</t>
   </si>
@@ -363,6 +363,18 @@
   <si>
     <t>normally like this…</t>
     <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8057: a9 80       LDA   #$80</t>
+  </si>
+  <si>
+    <t>8059: 8d 00 20    STA   $2000</t>
+  </si>
+  <si>
+    <t>805c: 8d 04 03    STA   $0304</t>
+  </si>
+  <si>
+    <t>805f: 4c 5f 80    JMP   $805f</t>
   </si>
 </sst>
 </file>
@@ -1894,13 +1906,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>626</xdr:row>
+      <xdr:row>632</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>672</xdr:row>
+      <xdr:row>678</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1941,13 +1953,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>653</xdr:row>
+      <xdr:row>659</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>659</xdr:row>
+      <xdr:row>665</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2003,6 +2015,419 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>692</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>737</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1371600" y="118338600"/>
+          <a:ext cx="12868275" cy="7715250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>715</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>721</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="角丸四角形吹き出し 32"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8562975" y="122348625"/>
+          <a:ext cx="1666875" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 28882"/>
+            <a:gd name="adj2" fmla="val -188461"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>nmi takes place</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> when </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>exec cycle=0</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>739</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>784</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1027" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1371600" y="126396750"/>
+          <a:ext cx="12868275" cy="7715250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>762</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>768</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="角丸四角形吹き出し 35"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9344025" y="130444875"/>
+          <a:ext cx="1666875" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 28882"/>
+            <a:gd name="adj2" fmla="val -188461"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>nmi takes place</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> when </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>exec cycle=1</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>602</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>608</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="角丸四角形吹き出し 36"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7400925" y="104013000"/>
+          <a:ext cx="1666875" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 116311"/>
+            <a:gd name="adj2" fmla="val -196153"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>why 994C???</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>659</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>665</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="角丸四角形吹き出し 37"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7467600" y="113747550"/>
+          <a:ext cx="1666875" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 116311"/>
+            <a:gd name="adj2" fmla="val -196153"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>return addr.</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>594</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>604</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="直線矢印コネクタ 39"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7734300" y="102698550"/>
+          <a:ext cx="409575" cy="1647825"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2605,9 +3030,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E626"/>
+  <dimension ref="A2:E690"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A572" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X601" sqref="X601"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -2796,9 +3223,54 @@
         <v>66</v>
       </c>
     </row>
-    <row r="626" spans="3:3">
-      <c r="C626" t="s">
+    <row r="573" spans="1:1">
+      <c r="A573" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="625" spans="1:3">
+      <c r="A625" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="632" spans="1:3">
+      <c r="C632" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="682" spans="2:2">
+      <c r="B682" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="683" spans="2:2">
+      <c r="B683" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="684" spans="2:2">
+      <c r="B684" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="687" spans="2:2">
+      <c r="B687" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="688" spans="2:2">
+      <c r="B688" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="689" spans="2:2">
+      <c r="B689" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="690" spans="2:2">
+      <c r="B690" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reset timing changed, nmi bug fixed.
</commit_message>
<xml_diff>
--- a/doc/mos6502-clock.xlsx
+++ b/doc/mos6502-clock.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="28035" windowHeight="13920" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="28035" windowHeight="13920" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="clock" sheetId="1" r:id="rId1"/>
     <sheet name="logic analyzer nmi debug" sheetId="4" r:id="rId2"/>
     <sheet name="debug emu" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="smb debug" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="102">
   <si>
     <t>---DE1 base clock 50 MHz</t>
   </si>
@@ -143,10 +143,6 @@
   </si>
   <si>
     <t>cpu clock=</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2a2cb</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -375,6 +371,112 @@
   </si>
   <si>
     <t>805f: 4c 5f 80    JMP   $805f</t>
+  </si>
+  <si>
+    <t>無限ループ</t>
+    <rPh sb="0" eb="2">
+      <t>ムゲン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8057: 4c 57 80    JMP   $8057</t>
+  </si>
+  <si>
+    <t>：</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>804f: ad 78 07    LDA   $0778</t>
+  </si>
+  <si>
+    <t>8052: 09 80       ORA   #$80</t>
+  </si>
+  <si>
+    <t>8054: 20 ed 8e    JSR   $8eed</t>
+  </si>
+  <si>
+    <t>8eed: 8d 00 20    STA   $2000</t>
+  </si>
+  <si>
+    <t>8ef0: 8d 78 07    STA   $0778</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8ef3: 60          RTS   </t>
+  </si>
+  <si>
+    <t>NMI</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8082: ad 78 07    LDA   $0778</t>
+  </si>
+  <si>
+    <t>8085: 29 7f       AND   #$7f</t>
+  </si>
+  <si>
+    <t>8087: 8d 78 07    STA   $0778</t>
+  </si>
+  <si>
+    <t>808a: 29 7e       AND   #$7e</t>
+  </si>
+  <si>
+    <t>808c: 8d 00 20    STA   $2000</t>
+  </si>
+  <si>
+    <t>RTI</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8178: ad 02 20    LDA   $2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">817b: 68          PLA   </t>
+  </si>
+  <si>
+    <t>817c: 09 80       ORA   #$80</t>
+  </si>
+  <si>
+    <t>817e: 8d 00 20    STA   $2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8181: 40          RTI   </t>
+  </si>
+  <si>
+    <t>不具合発生</t>
+    <rPh sb="0" eb="3">
+      <t>フグアイ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ハッセイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>clock=</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2FE4F</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2FE4F</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>→</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>5フレーム目で発生している</t>
+    <rPh sb="5" eb="6">
+      <t>メ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ハッセイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -422,12 +524,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -447,7 +555,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -473,6 +581,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2433,6 +2544,126 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1027" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="27603450"/>
+          <a:ext cx="18288000" cy="10287000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="角丸四角形吹き出し 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8677275" y="12296775"/>
+          <a:ext cx="1666875" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 116311"/>
+            <a:gd name="adj2" fmla="val -196153"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>wrong addr!!!</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
@@ -2721,7 +2952,7 @@
   <dimension ref="A3:J42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2858,12 +3089,12 @@
         <v>30</v>
       </c>
       <c r="I20" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="2:10">
       <c r="H21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="2:10">
@@ -2878,11 +3109,11 @@
         <v>19</v>
       </c>
       <c r="H23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I23" s="1">
         <f>HEX2DEC(I20)</f>
-        <v>172747</v>
+        <v>196175</v>
       </c>
     </row>
     <row r="24" spans="2:10">
@@ -2898,10 +3129,10 @@
       </c>
       <c r="I24">
         <f>ROUND(I23/C24,1)</f>
-        <v>4.9000000000000004</v>
+        <v>5.6</v>
       </c>
       <c r="J24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="2:10">
@@ -3032,7 +3263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E690"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A572" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A572" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="X601" sqref="X601"/>
     </sheetView>
   </sheetViews>
@@ -3045,15 +3276,15 @@
   <sheetData>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3061,72 +3292,72 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="116" spans="3:3">
       <c r="C116" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="117" spans="3:3">
       <c r="C117" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="118" spans="3:3">
@@ -3137,140 +3368,140 @@
     </row>
     <row r="150" spans="1:5">
       <c r="A150" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="151" spans="1:5">
       <c r="A151" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="152" spans="1:5">
       <c r="A152" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="153" spans="1:5">
       <c r="A153" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="155" spans="1:5">
       <c r="A155" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="158" spans="1:5">
       <c r="A158" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="159" spans="1:5">
       <c r="A159" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E159" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="160" spans="1:5">
       <c r="A160" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="42">
       <c r="C166" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="C167" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="270" spans="3:3">
       <c r="C270" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="372" spans="3:3" ht="42">
       <c r="C372" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="373" spans="3:3">
       <c r="C373" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="472" spans="3:3">
       <c r="C472" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="625" spans="1:3">
       <c r="A625" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="632" spans="1:3">
       <c r="C632" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="682" spans="2:2">
       <c r="B682" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="683" spans="2:2">
       <c r="B683" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="684" spans="2:2">
       <c r="B684" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="687" spans="2:2">
       <c r="B687" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="688" spans="2:2">
       <c r="B688" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="689" spans="2:2">
       <c r="B689" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="690" spans="2:2">
       <c r="B690" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -3296,67 +3527,67 @@
   <sheetData>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -3371,7 +3602,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -3392,13 +3623,277 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A3:K37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" t="s">
+        <v>77</v>
+      </c>
+      <c r="K6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" t="s">
+        <v>76</v>
+      </c>
+      <c r="K8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" t="s">
+        <v>76</v>
+      </c>
+      <c r="K9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="F10" t="s">
+        <v>76</v>
+      </c>
+      <c r="K10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="F11" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="K11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="F12" t="s">
+        <v>86</v>
+      </c>
+      <c r="K12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" t="s">
+        <v>87</v>
+      </c>
+      <c r="K13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" t="s">
+        <v>88</v>
+      </c>
+      <c r="K14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" t="s">
+        <v>89</v>
+      </c>
+      <c r="K15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" t="s">
+        <v>77</v>
+      </c>
+      <c r="K17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" t="s">
+        <v>77</v>
+      </c>
+      <c r="K18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="K20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
nmi wrong timing error...
</commit_message>
<xml_diff>
--- a/doc/mos6502-clock.xlsx
+++ b/doc/mos6502-clock.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="104">
   <si>
     <t>---DE1 base clock 50 MHz</t>
   </si>
@@ -453,28 +453,40 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>clock=</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>2FE4F</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>2FE4F</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>→</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>5フレーム目で発生している</t>
-    <rPh sb="5" eb="6">
-      <t>メ</t>
+    <t>A1CDB</t>
+  </si>
+  <si>
+    <t>99423</t>
+  </si>
+  <si>
+    <t>次の間でおかしくなる</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
     </rPh>
-    <rPh sb="7" eb="9">
-      <t>ハッセイ</t>
+    <rPh sb="2" eb="3">
+      <t>アイダ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>&gt;&gt;　9e939</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>でおかしくなっている</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>正しい場合</t>
+    <rPh sb="0" eb="1">
+      <t>タダ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>バアイ</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -2550,18 +2562,18 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>98</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1027" name="Picture 3"/>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2575,7 +2587,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="27603450"/>
+          <a:off x="0" y="5314950"/>
           <a:ext cx="18288000" cy="10287000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2596,30 +2608,30 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="角丸四角形吹き出し 4"/>
+        <xdr:cNvPr id="6" name="角丸四角形吹き出し 5"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8677275" y="12296775"/>
-          <a:ext cx="1666875" cy="990600"/>
+          <a:off x="8810625" y="10096500"/>
+          <a:ext cx="1504950" cy="876300"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 116311"/>
-            <a:gd name="adj2" fmla="val -196153"/>
+            <a:gd name="adj1" fmla="val 73471"/>
+            <a:gd name="adj2" fmla="val -112500"/>
             <a:gd name="adj3" fmla="val 16667"/>
           </a:avLst>
         </a:prstGeom>
@@ -2644,17 +2656,370 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="1">
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>RTI</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>の戻りがおかしい</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:schemeClr val="dk1"/>
               </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>wrong addr!!!</a:t>
+            <a:t>8057</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1">
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>に戻らないといけない</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
             <a:solidFill>
-              <a:srgbClr val="FF0000"/>
+              <a:schemeClr val="dk1"/>
             </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="16116300"/>
+          <a:ext cx="18288000" cy="10287000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="角丸四角形吹き出し 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10972800" y="20926425"/>
+          <a:ext cx="1504950" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 73471"/>
+            <a:gd name="adj2" fmla="val -112500"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>8058</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>を</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>push</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>している</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>219</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1028" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="27260550"/>
+          <a:ext cx="18288000" cy="10287000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>191</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="角丸四角形吹き出し 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9420225" y="31994475"/>
+          <a:ext cx="1504950" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 73471"/>
+            <a:gd name="adj2" fmla="val -112500"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>8057</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>を</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>push</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>している</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -2952,7 +3317,7 @@
   <dimension ref="A3:J42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3089,7 +3454,7 @@
         <v>30</v>
       </c>
       <c r="I20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="2:10">
@@ -3224,29 +3589,29 @@
     <row r="40" spans="2:5">
       <c r="B40" t="str">
         <f>E40&amp;"回目のvblankは"</f>
-        <v>8回目のvblankは</v>
+        <v>17回目のvblankは</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>29</v>
       </c>
       <c r="E40" s="3">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="2:5">
       <c r="C41" s="6">
         <f>$C$29+$C$24*(E40-1)</f>
-        <v>277747</v>
+        <v>592747</v>
       </c>
       <c r="D41" s="1">
         <f>C41*$D$13</f>
-        <v>133318560</v>
+        <v>284518560</v>
       </c>
     </row>
     <row r="42" spans="2:5">
       <c r="C42" t="str">
         <f>DEC2HEX(C41)</f>
-        <v>43CF3</v>
+        <v>90B6B</v>
       </c>
       <c r="D42" t="s">
         <v>26</v>
@@ -3623,10 +3988,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:K37"/>
+  <dimension ref="A3:K158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A158" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A159" sqref="A159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3838,57 +4203,27 @@
       </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" t="s">
-        <v>97</v>
-      </c>
       <c r="B28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="D29" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" t="s">
-        <v>100</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="F29" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>76</v>
+      <c r="G29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merge cpu test all
</commit_message>
<xml_diff>
--- a/doc/mos6502-clock.xlsx
+++ b/doc/mos6502-clock.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="28035" windowHeight="13920" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="405" windowWidth="27795" windowHeight="12285" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="clock" sheetId="1" r:id="rId1"/>
     <sheet name="logic analyzer nmi debug" sheetId="4" r:id="rId2"/>
     <sheet name="debug emu" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="smb debug" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="104">
   <si>
     <t>---DE1 base clock 50 MHz</t>
   </si>
@@ -143,10 +143,6 @@
   </si>
   <si>
     <t>cpu clock=</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2a2cb</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -375,6 +371,124 @@
   </si>
   <si>
     <t>805f: 4c 5f 80    JMP   $805f</t>
+  </si>
+  <si>
+    <t>無限ループ</t>
+    <rPh sb="0" eb="2">
+      <t>ムゲン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8057: 4c 57 80    JMP   $8057</t>
+  </si>
+  <si>
+    <t>：</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>804f: ad 78 07    LDA   $0778</t>
+  </si>
+  <si>
+    <t>8052: 09 80       ORA   #$80</t>
+  </si>
+  <si>
+    <t>8054: 20 ed 8e    JSR   $8eed</t>
+  </si>
+  <si>
+    <t>8eed: 8d 00 20    STA   $2000</t>
+  </si>
+  <si>
+    <t>8ef0: 8d 78 07    STA   $0778</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8ef3: 60          RTS   </t>
+  </si>
+  <si>
+    <t>NMI</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8082: ad 78 07    LDA   $0778</t>
+  </si>
+  <si>
+    <t>8085: 29 7f       AND   #$7f</t>
+  </si>
+  <si>
+    <t>8087: 8d 78 07    STA   $0778</t>
+  </si>
+  <si>
+    <t>808a: 29 7e       AND   #$7e</t>
+  </si>
+  <si>
+    <t>808c: 8d 00 20    STA   $2000</t>
+  </si>
+  <si>
+    <t>RTI</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8178: ad 02 20    LDA   $2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">817b: 68          PLA   </t>
+  </si>
+  <si>
+    <t>817c: 09 80       ORA   #$80</t>
+  </si>
+  <si>
+    <t>817e: 8d 00 20    STA   $2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8181: 40          RTI   </t>
+  </si>
+  <si>
+    <t>不具合発生</t>
+    <rPh sb="0" eb="3">
+      <t>フグアイ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ハッセイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2FE4F</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>A1CDB</t>
+  </si>
+  <si>
+    <t>99423</t>
+  </si>
+  <si>
+    <t>次の間でおかしくなる</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>アイダ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>&gt;&gt;　9e939</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>でおかしくなっている</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>正しい場合</t>
+    <rPh sb="0" eb="1">
+      <t>タダ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -422,12 +536,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -447,7 +567,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -473,6 +593,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2433,6 +2556,479 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="5314950"/>
+          <a:ext cx="18288000" cy="10287000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="角丸四角形吹き出し 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8810625" y="10096500"/>
+          <a:ext cx="1504950" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 73471"/>
+            <a:gd name="adj2" fmla="val -112500"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>RTI</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>の戻りがおかしい</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>8057</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>に戻らないといけない</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="16278225"/>
+          <a:ext cx="18288000" cy="10287000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="角丸四角形吹き出し 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10915650" y="21974175"/>
+          <a:ext cx="1504950" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 107015"/>
+            <a:gd name="adj2" fmla="val -158152"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>8058</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>を</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>push</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>している</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1028" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1628775" y="27565350"/>
+          <a:ext cx="18288000" cy="10287000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>195</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="角丸四角形吹き出し 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9439275" y="32699325"/>
+          <a:ext cx="1504950" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 73471"/>
+            <a:gd name="adj2" fmla="val -112500"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>8057</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>を</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>push</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>している</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
@@ -2720,9 +3316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:J42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -2858,12 +3452,12 @@
         <v>30</v>
       </c>
       <c r="I20" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="2:10">
       <c r="H21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="2:10">
@@ -2878,11 +3472,11 @@
         <v>19</v>
       </c>
       <c r="H23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I23" s="1">
         <f>HEX2DEC(I20)</f>
-        <v>172747</v>
+        <v>196175</v>
       </c>
     </row>
     <row r="24" spans="2:10">
@@ -2898,10 +3492,10 @@
       </c>
       <c r="I24">
         <f>ROUND(I23/C24,1)</f>
-        <v>4.9000000000000004</v>
+        <v>5.6</v>
       </c>
       <c r="J24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="2:10">
@@ -2993,29 +3587,29 @@
     <row r="40" spans="2:5">
       <c r="B40" t="str">
         <f>E40&amp;"回目のvblankは"</f>
-        <v>8回目のvblankは</v>
+        <v>17回目のvblankは</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>29</v>
       </c>
       <c r="E40" s="3">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="2:5">
       <c r="C41" s="6">
         <f>$C$29+$C$24*(E40-1)</f>
-        <v>277747</v>
+        <v>592747</v>
       </c>
       <c r="D41" s="1">
         <f>C41*$D$13</f>
-        <v>133318560</v>
+        <v>284518560</v>
       </c>
     </row>
     <row r="42" spans="2:5">
       <c r="C42" t="str">
         <f>DEC2HEX(C41)</f>
-        <v>43CF3</v>
+        <v>90B6B</v>
       </c>
       <c r="D42" t="s">
         <v>26</v>
@@ -3032,9 +3626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E690"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A572" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X601" sqref="X601"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -3045,15 +3637,15 @@
   <sheetData>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3061,72 +3653,72 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="116" spans="3:3">
       <c r="C116" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="117" spans="3:3">
       <c r="C117" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="118" spans="3:3">
@@ -3137,140 +3729,140 @@
     </row>
     <row r="150" spans="1:5">
       <c r="A150" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="151" spans="1:5">
       <c r="A151" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="152" spans="1:5">
       <c r="A152" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="153" spans="1:5">
       <c r="A153" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="155" spans="1:5">
       <c r="A155" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="158" spans="1:5">
       <c r="A158" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="159" spans="1:5">
       <c r="A159" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E159" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="160" spans="1:5">
       <c r="A160" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="42">
       <c r="C166" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="C167" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="270" spans="3:3">
       <c r="C270" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="372" spans="3:3" ht="42">
       <c r="C372" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="373" spans="3:3">
       <c r="C373" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="472" spans="3:3">
       <c r="C472" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="625" spans="1:3">
       <c r="A625" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="632" spans="1:3">
       <c r="C632" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="682" spans="2:2">
       <c r="B682" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="683" spans="2:2">
       <c r="B683" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="684" spans="2:2">
       <c r="B684" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="687" spans="2:2">
       <c r="B687" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="688" spans="2:2">
       <c r="B688" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="689" spans="2:2">
       <c r="B689" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="690" spans="2:2">
       <c r="B690" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -3285,9 +3877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -3296,67 +3886,67 @@
   <sheetData>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -3371,7 +3961,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -3392,13 +3982,248 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A3:N158"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" t="s">
+        <v>77</v>
+      </c>
+      <c r="K6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" t="s">
+        <v>76</v>
+      </c>
+      <c r="K8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" t="s">
+        <v>76</v>
+      </c>
+      <c r="K9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="F10" t="s">
+        <v>76</v>
+      </c>
+      <c r="K10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="F11" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="K11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="F12" t="s">
+        <v>86</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" t="s">
+        <v>87</v>
+      </c>
+      <c r="K13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" t="s">
+        <v>88</v>
+      </c>
+      <c r="K14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" t="s">
+        <v>89</v>
+      </c>
+      <c r="K15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" t="s">
+        <v>77</v>
+      </c>
+      <c r="K17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" t="s">
+        <v>77</v>
+      </c>
+      <c r="K18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="K20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="B28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="D29" t="s">
+        <v>98</v>
+      </c>
+      <c r="F29" t="s">
+        <v>101</v>
+      </c>
+      <c r="G29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ppu ram timing changed, but not working yet...
</commit_message>
<xml_diff>
--- a/doc/mos6502-clock.xlsx
+++ b/doc/mos6502-clock.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="405" windowWidth="27795" windowHeight="12285"/>
+    <workbookView xWindow="600" yWindow="405" windowWidth="27795" windowHeight="12285" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="clock" sheetId="1" r:id="rId1"/>
-    <sheet name="logic analyzer nmi debug" sheetId="4" r:id="rId2"/>
-    <sheet name="debug emu" sheetId="2" r:id="rId3"/>
-    <sheet name="smb debug" sheetId="3" r:id="rId4"/>
+    <sheet name="clock diiagram" sheetId="5" r:id="rId2"/>
+    <sheet name="logic analyzer nmi debug" sheetId="4" r:id="rId3"/>
+    <sheet name="debug emu" sheetId="2" r:id="rId4"/>
+    <sheet name="smb debug" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="109">
   <si>
     <t>---DE1 base clock 50 MHz</t>
   </si>
@@ -496,6 +497,18 @@
   </si>
   <si>
     <t xml:space="preserve">    --emu ppu clock = base clock / 4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CPU</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>PPU</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>VGA</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -617,6 +630,4307 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="20" name="グループ化 19"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="876300" y="2057400"/>
+          <a:ext cx="5257800" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="5" name="直線コネクタ 4"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="7" name="直線コネクタ 6"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="8" name="直線コネクタ 7"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="10" name="直線コネクタ 9"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="13" name="直線コネクタ 12"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="32" name="グループ化 31"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="876301" y="685800"/>
+          <a:ext cx="438150" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="33" name="直線コネクタ 32"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="34" name="直線コネクタ 33"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="35" name="直線コネクタ 34"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="36" name="直線コネクタ 35"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="37" name="直線コネクタ 36"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="38" name="グループ化 37"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="876300" y="3600450"/>
+          <a:ext cx="3505200" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="39" name="直線コネクタ 38"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="40" name="直線コネクタ 39"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="41" name="直線コネクタ 40"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="42" name="直線コネクタ 41"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="43" name="直線コネクタ 42"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="44" name="グループ化 43"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1314450" y="685800"/>
+          <a:ext cx="438150" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="45" name="直線コネクタ 44"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="46" name="直線コネクタ 45"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="47" name="直線コネクタ 46"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="48" name="直線コネクタ 47"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="49" name="直線コネクタ 48"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="50" name="グループ化 49"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1752600" y="685800"/>
+          <a:ext cx="438150" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="51" name="直線コネクタ 50"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="52" name="直線コネクタ 51"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="53" name="直線コネクタ 52"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="54" name="直線コネクタ 53"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="55" name="直線コネクタ 54"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="56" name="グループ化 55"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2190750" y="685800"/>
+          <a:ext cx="438150" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="57" name="直線コネクタ 56"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="58" name="直線コネクタ 57"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="59" name="直線コネクタ 58"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="60" name="直線コネクタ 59"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="61" name="直線コネクタ 60"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="62" name="グループ化 61"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2628900" y="685800"/>
+          <a:ext cx="438150" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="63" name="直線コネクタ 62"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="64" name="直線コネクタ 63"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="65" name="直線コネクタ 64"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="66" name="直線コネクタ 65"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="67" name="直線コネクタ 66"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="74" name="グループ化 73"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3067050" y="685800"/>
+          <a:ext cx="438150" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="75" name="直線コネクタ 74"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="76" name="直線コネクタ 75"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="77" name="直線コネクタ 76"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="78" name="直線コネクタ 77"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="79" name="直線コネクタ 78"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="80" name="グループ化 79"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3505199" y="685800"/>
+          <a:ext cx="438150" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="81" name="直線コネクタ 80"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="82" name="直線コネクタ 81"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="83" name="直線コネクタ 82"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="84" name="直線コネクタ 83"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="85" name="直線コネクタ 84"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="86" name="グループ化 85"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3943349" y="685800"/>
+          <a:ext cx="438150" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="87" name="直線コネクタ 86"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="88" name="直線コネクタ 87"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="89" name="直線コネクタ 88"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="90" name="直線コネクタ 89"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="91" name="直線コネクタ 90"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="92" name="グループ化 91"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4381499" y="685800"/>
+          <a:ext cx="438150" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="93" name="直線コネクタ 92"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="94" name="直線コネクタ 93"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="95" name="直線コネクタ 94"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="96" name="直線コネクタ 95"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="97" name="直線コネクタ 96"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="98" name="グループ化 97"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4819649" y="685800"/>
+          <a:ext cx="438150" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="99" name="直線コネクタ 98"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="100" name="直線コネクタ 99"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="101" name="直線コネクタ 100"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="102" name="直線コネクタ 101"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="103" name="直線コネクタ 102"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="104" name="グループ化 103"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4381500" y="3600450"/>
+          <a:ext cx="3505200" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="105" name="直線コネクタ 104"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="106" name="直線コネクタ 105"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="107" name="直線コネクタ 106"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="108" name="直線コネクタ 107"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="109" name="直線コネクタ 108"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="110" name="グループ化 109"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="7886700" y="3600450"/>
+          <a:ext cx="3505200" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="111" name="直線コネクタ 110"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="112" name="直線コネクタ 111"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="113" name="直線コネクタ 112"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="114" name="直線コネクタ 113"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="115" name="直線コネクタ 114"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="116" name="グループ化 115"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="6134100" y="2057400"/>
+          <a:ext cx="5257800" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="117" name="直線コネクタ 116"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="118" name="直線コネクタ 117"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="119" name="直線コネクタ 118"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="120" name="直線コネクタ 119"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="121" name="直線コネクタ 120"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="128" name="グループ化 127"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="876300" y="5143500"/>
+          <a:ext cx="876300" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="129" name="直線コネクタ 128"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="130" name="直線コネクタ 129"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="131" name="直線コネクタ 130"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="132" name="直線コネクタ 131"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="133" name="直線コネクタ 132"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="146" name="グループ化 145"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="876300" y="6515100"/>
+          <a:ext cx="1752600" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="147" name="直線コネクタ 146"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="148" name="直線コネクタ 147"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="149" name="直線コネクタ 148"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="150" name="直線コネクタ 149"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="151" name="直線コネクタ 150"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="152" name="グループ化 151"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2628900" y="6515100"/>
+          <a:ext cx="1752600" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="153" name="直線コネクタ 152"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="154" name="直線コネクタ 153"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="155" name="直線コネクタ 154"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="156" name="直線コネクタ 155"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="157" name="直線コネクタ 156"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="158" name="グループ化 157"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4381500" y="6515100"/>
+          <a:ext cx="1752600" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="159" name="直線コネクタ 158"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="160" name="直線コネクタ 159"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="161" name="直線コネクタ 160"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="162" name="直線コネクタ 161"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="163" name="直線コネクタ 162"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="164" name="グループ化 163"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1752600" y="5143500"/>
+          <a:ext cx="876300" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="165" name="直線コネクタ 164"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="166" name="直線コネクタ 165"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="167" name="直線コネクタ 166"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="168" name="直線コネクタ 167"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="169" name="直線コネクタ 168"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="170" name="グループ化 169"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2628900" y="5143500"/>
+          <a:ext cx="876300" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="171" name="直線コネクタ 170"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="172" name="直線コネクタ 171"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="173" name="直線コネクタ 172"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="174" name="直線コネクタ 173"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="175" name="直線コネクタ 174"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="176" name="グループ化 175"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3505200" y="5143500"/>
+          <a:ext cx="876300" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="177" name="直線コネクタ 176"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="178" name="直線コネクタ 177"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="179" name="直線コネクタ 178"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="180" name="直線コネクタ 179"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="181" name="直線コネクタ 180"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="194" name="グループ化 193"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4381500" y="5143500"/>
+          <a:ext cx="876300" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="195" name="直線コネクタ 194"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="196" name="直線コネクタ 195"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="197" name="直線コネクタ 196"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="198" name="直線コネクタ 197"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="199" name="直線コネクタ 198"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="200" name="グループ化 199"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5257800" y="5143500"/>
+          <a:ext cx="876300" cy="685800"/>
+          <a:chOff x="876300" y="2743200"/>
+          <a:chExt cx="5257800" cy="685800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="201" name="直線コネクタ 200"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3429000"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="202" name="直線コネクタ 201"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="2628900" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="203" name="直線コネクタ 202"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3505200" y="2743200"/>
+            <a:ext cx="0" cy="685800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="204" name="直線コネクタ 203"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="876300" y="3086100"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="205" name="直線コネクタ 204"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6134100" y="2743200"/>
+            <a:ext cx="0" cy="342900"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2564,7 +6878,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3324,7 +7638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -3653,6 +7967,478 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3:AE40"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="AT34" sqref="AT34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="3" spans="1:31">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <v>7</v>
+      </c>
+      <c r="L3">
+        <v>8</v>
+      </c>
+      <c r="M3">
+        <v>9</v>
+      </c>
+      <c r="N3">
+        <v>10</v>
+      </c>
+      <c r="O3">
+        <v>11</v>
+      </c>
+      <c r="P3">
+        <v>12</v>
+      </c>
+      <c r="Q3">
+        <v>13</v>
+      </c>
+      <c r="R3">
+        <v>14</v>
+      </c>
+      <c r="S3">
+        <v>15</v>
+      </c>
+      <c r="T3">
+        <v>16</v>
+      </c>
+      <c r="U3">
+        <v>17</v>
+      </c>
+      <c r="V3">
+        <v>18</v>
+      </c>
+      <c r="W3">
+        <v>19</v>
+      </c>
+      <c r="X3">
+        <v>20</v>
+      </c>
+      <c r="Y3">
+        <v>21</v>
+      </c>
+      <c r="Z3">
+        <v>22</v>
+      </c>
+      <c r="AA3">
+        <v>23</v>
+      </c>
+      <c r="AB3">
+        <v>24</v>
+      </c>
+      <c r="AC3">
+        <v>25</v>
+      </c>
+      <c r="AD3">
+        <v>26</v>
+      </c>
+      <c r="AE3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31">
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>7</v>
+      </c>
+      <c r="L11">
+        <v>8</v>
+      </c>
+      <c r="M11">
+        <v>9</v>
+      </c>
+      <c r="N11">
+        <v>10</v>
+      </c>
+      <c r="O11">
+        <v>11</v>
+      </c>
+      <c r="P11">
+        <v>12</v>
+      </c>
+      <c r="Q11">
+        <v>13</v>
+      </c>
+      <c r="R11">
+        <v>14</v>
+      </c>
+      <c r="S11">
+        <v>15</v>
+      </c>
+      <c r="T11">
+        <v>16</v>
+      </c>
+      <c r="U11">
+        <v>17</v>
+      </c>
+      <c r="V11">
+        <v>18</v>
+      </c>
+      <c r="W11">
+        <v>19</v>
+      </c>
+      <c r="X11">
+        <v>20</v>
+      </c>
+      <c r="Y11">
+        <v>21</v>
+      </c>
+      <c r="Z11">
+        <v>22</v>
+      </c>
+      <c r="AA11">
+        <v>23</v>
+      </c>
+      <c r="AB11">
+        <v>24</v>
+      </c>
+      <c r="AC11">
+        <v>25</v>
+      </c>
+      <c r="AD11">
+        <v>26</v>
+      </c>
+      <c r="AE11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31">
+      <c r="B14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="2:31">
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <v>6</v>
+      </c>
+      <c r="K19">
+        <v>7</v>
+      </c>
+      <c r="L19">
+        <v>8</v>
+      </c>
+      <c r="M19">
+        <v>9</v>
+      </c>
+      <c r="N19">
+        <v>10</v>
+      </c>
+      <c r="O19">
+        <v>11</v>
+      </c>
+      <c r="P19">
+        <v>12</v>
+      </c>
+      <c r="Q19">
+        <v>13</v>
+      </c>
+      <c r="R19">
+        <v>14</v>
+      </c>
+      <c r="S19">
+        <v>15</v>
+      </c>
+      <c r="T19">
+        <v>16</v>
+      </c>
+      <c r="U19">
+        <v>17</v>
+      </c>
+      <c r="V19">
+        <v>18</v>
+      </c>
+      <c r="W19">
+        <v>19</v>
+      </c>
+      <c r="X19">
+        <v>20</v>
+      </c>
+      <c r="Y19">
+        <v>21</v>
+      </c>
+      <c r="Z19">
+        <v>22</v>
+      </c>
+      <c r="AA19">
+        <v>23</v>
+      </c>
+      <c r="AB19">
+        <v>24</v>
+      </c>
+      <c r="AC19">
+        <v>25</v>
+      </c>
+      <c r="AD19">
+        <v>26</v>
+      </c>
+      <c r="AE19">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="2:31">
+      <c r="B23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="2:31">
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29">
+        <v>4</v>
+      </c>
+      <c r="I29">
+        <v>5</v>
+      </c>
+      <c r="J29">
+        <v>6</v>
+      </c>
+      <c r="K29">
+        <v>7</v>
+      </c>
+      <c r="L29">
+        <v>8</v>
+      </c>
+      <c r="M29">
+        <v>9</v>
+      </c>
+      <c r="N29">
+        <v>10</v>
+      </c>
+      <c r="O29">
+        <v>11</v>
+      </c>
+      <c r="P29">
+        <v>12</v>
+      </c>
+      <c r="Q29">
+        <v>13</v>
+      </c>
+      <c r="R29">
+        <v>14</v>
+      </c>
+      <c r="S29">
+        <v>15</v>
+      </c>
+      <c r="T29">
+        <v>16</v>
+      </c>
+      <c r="U29">
+        <v>17</v>
+      </c>
+      <c r="V29">
+        <v>18</v>
+      </c>
+      <c r="W29">
+        <v>19</v>
+      </c>
+      <c r="X29">
+        <v>20</v>
+      </c>
+      <c r="Y29">
+        <v>21</v>
+      </c>
+      <c r="Z29">
+        <v>22</v>
+      </c>
+      <c r="AA29">
+        <v>23</v>
+      </c>
+      <c r="AB29">
+        <v>24</v>
+      </c>
+      <c r="AC29">
+        <v>25</v>
+      </c>
+      <c r="AD29">
+        <v>26</v>
+      </c>
+      <c r="AE29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="2:31">
+      <c r="B32" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="2:31">
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+      <c r="H37">
+        <v>4</v>
+      </c>
+      <c r="I37">
+        <v>5</v>
+      </c>
+      <c r="J37">
+        <v>6</v>
+      </c>
+      <c r="K37">
+        <v>7</v>
+      </c>
+      <c r="L37">
+        <v>8</v>
+      </c>
+      <c r="M37">
+        <v>9</v>
+      </c>
+      <c r="N37">
+        <v>10</v>
+      </c>
+      <c r="O37">
+        <v>11</v>
+      </c>
+      <c r="P37">
+        <v>12</v>
+      </c>
+      <c r="Q37">
+        <v>13</v>
+      </c>
+      <c r="R37">
+        <v>14</v>
+      </c>
+      <c r="S37">
+        <v>15</v>
+      </c>
+      <c r="T37">
+        <v>16</v>
+      </c>
+      <c r="U37">
+        <v>17</v>
+      </c>
+      <c r="V37">
+        <v>18</v>
+      </c>
+      <c r="W37">
+        <v>19</v>
+      </c>
+      <c r="X37">
+        <v>20</v>
+      </c>
+      <c r="Y37">
+        <v>21</v>
+      </c>
+      <c r="Z37">
+        <v>22</v>
+      </c>
+      <c r="AA37">
+        <v>23</v>
+      </c>
+      <c r="AB37">
+        <v>24</v>
+      </c>
+      <c r="AC37">
+        <v>25</v>
+      </c>
+      <c r="AD37">
+        <v>26</v>
+      </c>
+      <c r="AE37">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="2:31">
+      <c r="B40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E690"/>
   <sheetViews>
@@ -3903,7 +8689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:B26"/>
   <sheetViews>
@@ -4010,7 +8796,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:N158"/>
   <sheetViews>

</xml_diff>

<commit_message>
bg pattern ok on rtl.
</commit_message>
<xml_diff>
--- a/doc/mos6502-clock.xlsx
+++ b/doc/mos6502-clock.xlsx
@@ -14,12 +14,12 @@
     <sheet name="debug emu" sheetId="2" r:id="rId5"/>
     <sheet name="smb debug" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725" calcMode="manual"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="281">
   <si>
     <t>---DE1 base clock 50 MHz</t>
   </si>
@@ -1013,19 +1013,31 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>REG_SET</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>reg set</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>R0</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>R1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>cs out</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>REG_SET</t>
+    <t>cs clr</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>reg set</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>cs clr</t>
+    <t>ptn shift</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1619,10 +1631,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
@@ -8835,14 +8847,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:BH252"/>
+  <dimension ref="A2:BH248"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E233" activePane="bottomRight" state="frozenSplit"/>
       <selection activeCell="A21" sqref="A21"/>
       <selection pane="topRight" activeCell="E21" sqref="E21"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="F253" sqref="F253"/>
+      <selection pane="bottomRight" activeCell="I250" sqref="I250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -8989,76 +9001,76 @@
     <row r="21" spans="1:60">
       <c r="A21" s="2"/>
       <c r="B21" s="1"/>
-      <c r="E21" s="45" t="s">
+      <c r="E21" s="44" t="s">
         <v>169</v>
       </c>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="45" t="s">
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="44" t="s">
         <v>170</v>
       </c>
-      <c r="N21" s="45"/>
-      <c r="O21" s="45"/>
-      <c r="P21" s="45"/>
-      <c r="Q21" s="45"/>
-      <c r="R21" s="45"/>
-      <c r="S21" s="45"/>
-      <c r="T21" s="45"/>
-      <c r="U21" s="45" t="s">
+      <c r="N21" s="44"/>
+      <c r="O21" s="44"/>
+      <c r="P21" s="44"/>
+      <c r="Q21" s="44"/>
+      <c r="R21" s="44"/>
+      <c r="S21" s="44"/>
+      <c r="T21" s="44"/>
+      <c r="U21" s="44" t="s">
         <v>171</v>
       </c>
-      <c r="V21" s="45"/>
-      <c r="W21" s="45"/>
-      <c r="X21" s="45"/>
-      <c r="Y21" s="45"/>
-      <c r="Z21" s="45"/>
-      <c r="AA21" s="45"/>
-      <c r="AB21" s="45"/>
-      <c r="AC21" s="45" t="s">
+      <c r="V21" s="44"/>
+      <c r="W21" s="44"/>
+      <c r="X21" s="44"/>
+      <c r="Y21" s="44"/>
+      <c r="Z21" s="44"/>
+      <c r="AA21" s="44"/>
+      <c r="AB21" s="44"/>
+      <c r="AC21" s="44" t="s">
         <v>172</v>
       </c>
-      <c r="AD21" s="45"/>
-      <c r="AE21" s="45"/>
-      <c r="AF21" s="45"/>
-      <c r="AG21" s="45"/>
-      <c r="AH21" s="45"/>
-      <c r="AI21" s="45"/>
-      <c r="AJ21" s="45"/>
-      <c r="AK21" s="45" t="s">
+      <c r="AD21" s="44"/>
+      <c r="AE21" s="44"/>
+      <c r="AF21" s="44"/>
+      <c r="AG21" s="44"/>
+      <c r="AH21" s="44"/>
+      <c r="AI21" s="44"/>
+      <c r="AJ21" s="44"/>
+      <c r="AK21" s="44" t="s">
         <v>173</v>
       </c>
-      <c r="AL21" s="45"/>
-      <c r="AM21" s="45"/>
-      <c r="AN21" s="45"/>
-      <c r="AO21" s="45"/>
-      <c r="AP21" s="45"/>
-      <c r="AQ21" s="45"/>
-      <c r="AR21" s="45"/>
-      <c r="AS21" s="45" t="s">
+      <c r="AL21" s="44"/>
+      <c r="AM21" s="44"/>
+      <c r="AN21" s="44"/>
+      <c r="AO21" s="44"/>
+      <c r="AP21" s="44"/>
+      <c r="AQ21" s="44"/>
+      <c r="AR21" s="44"/>
+      <c r="AS21" s="44" t="s">
         <v>174</v>
       </c>
-      <c r="AT21" s="45"/>
-      <c r="AU21" s="45"/>
-      <c r="AV21" s="45"/>
-      <c r="AW21" s="45"/>
-      <c r="AX21" s="45"/>
-      <c r="AY21" s="45"/>
-      <c r="AZ21" s="45"/>
-      <c r="BA21" s="45" t="s">
+      <c r="AT21" s="44"/>
+      <c r="AU21" s="44"/>
+      <c r="AV21" s="44"/>
+      <c r="AW21" s="44"/>
+      <c r="AX21" s="44"/>
+      <c r="AY21" s="44"/>
+      <c r="AZ21" s="44"/>
+      <c r="BA21" s="44" t="s">
         <v>190</v>
       </c>
-      <c r="BB21" s="45"/>
-      <c r="BC21" s="45"/>
-      <c r="BD21" s="45"/>
-      <c r="BE21" s="45"/>
-      <c r="BF21" s="45"/>
-      <c r="BG21" s="45"/>
-      <c r="BH21" s="45"/>
+      <c r="BB21" s="44"/>
+      <c r="BC21" s="44"/>
+      <c r="BD21" s="44"/>
+      <c r="BE21" s="44"/>
+      <c r="BF21" s="44"/>
+      <c r="BG21" s="44"/>
+      <c r="BH21" s="44"/>
     </row>
     <row r="22" spans="1:60">
       <c r="E22" s="29" t="str">
@@ -9351,26 +9363,26 @@
       <c r="C24" t="s">
         <v>143</v>
       </c>
-      <c r="E24" s="45" t="s">
+      <c r="E24" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="45"/>
-      <c r="M24" s="45" t="s">
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="N24" s="45"/>
-      <c r="O24" s="45"/>
-      <c r="P24" s="45"/>
-      <c r="Q24" s="45"/>
-      <c r="R24" s="45"/>
-      <c r="S24" s="45"/>
-      <c r="T24" s="45"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
+      <c r="P24" s="44"/>
+      <c r="Q24" s="44"/>
+      <c r="R24" s="44"/>
+      <c r="S24" s="44"/>
+      <c r="T24" s="44"/>
       <c r="U24" s="23"/>
       <c r="V24" s="21"/>
       <c r="W24" s="21"/>
@@ -9724,26 +9736,26 @@
       <c r="C30" t="s">
         <v>144</v>
       </c>
-      <c r="E30" s="45" t="s">
+      <c r="E30" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
-      <c r="K30" s="45"/>
-      <c r="L30" s="45"/>
-      <c r="M30" s="45" t="s">
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="44"/>
+      <c r="M30" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="N30" s="45"/>
-      <c r="O30" s="45"/>
-      <c r="P30" s="45"/>
-      <c r="Q30" s="45"/>
-      <c r="R30" s="45"/>
-      <c r="S30" s="45"/>
-      <c r="T30" s="45"/>
+      <c r="N30" s="44"/>
+      <c r="O30" s="44"/>
+      <c r="P30" s="44"/>
+      <c r="Q30" s="44"/>
+      <c r="R30" s="44"/>
+      <c r="S30" s="44"/>
+      <c r="T30" s="44"/>
       <c r="U30" s="23"/>
       <c r="V30" s="21"/>
       <c r="W30" s="21"/>
@@ -10105,36 +10117,36 @@
       <c r="C36" t="s">
         <v>145</v>
       </c>
-      <c r="E36" s="45" t="s">
+      <c r="E36" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45" t="s">
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="44"/>
+      <c r="L36" s="44"/>
+      <c r="M36" s="44" t="s">
         <v>184</v>
       </c>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="45"/>
-      <c r="R36" s="45"/>
-      <c r="S36" s="45"/>
-      <c r="T36" s="45"/>
-      <c r="U36" s="45" t="s">
+      <c r="N36" s="44"/>
+      <c r="O36" s="44"/>
+      <c r="P36" s="44"/>
+      <c r="Q36" s="44"/>
+      <c r="R36" s="44"/>
+      <c r="S36" s="44"/>
+      <c r="T36" s="44"/>
+      <c r="U36" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="V36" s="45"/>
-      <c r="W36" s="45"/>
-      <c r="X36" s="45"/>
-      <c r="Y36" s="45"/>
-      <c r="Z36" s="45"/>
-      <c r="AA36" s="45"/>
-      <c r="AB36" s="45"/>
+      <c r="V36" s="44"/>
+      <c r="W36" s="44"/>
+      <c r="X36" s="44"/>
+      <c r="Y36" s="44"/>
+      <c r="Z36" s="44"/>
+      <c r="AA36" s="44"/>
+      <c r="AB36" s="44"/>
       <c r="AC36" s="23"/>
       <c r="AD36" s="21"/>
       <c r="AE36" s="21"/>
@@ -10493,46 +10505,46 @@
       <c r="C42" t="s">
         <v>146</v>
       </c>
-      <c r="E42" s="45" t="s">
+      <c r="E42" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="45" t="s">
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="44"/>
+      <c r="K42" s="44"/>
+      <c r="L42" s="44"/>
+      <c r="M42" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="45"/>
-      <c r="R42" s="45"/>
-      <c r="S42" s="45"/>
-      <c r="T42" s="45"/>
-      <c r="U42" s="45" t="s">
+      <c r="N42" s="44"/>
+      <c r="O42" s="44"/>
+      <c r="P42" s="44"/>
+      <c r="Q42" s="44"/>
+      <c r="R42" s="44"/>
+      <c r="S42" s="44"/>
+      <c r="T42" s="44"/>
+      <c r="U42" s="44" t="s">
         <v>177</v>
       </c>
-      <c r="V42" s="45"/>
-      <c r="W42" s="45"/>
-      <c r="X42" s="45"/>
-      <c r="Y42" s="45"/>
-      <c r="Z42" s="45"/>
-      <c r="AA42" s="45"/>
-      <c r="AB42" s="45"/>
-      <c r="AC42" s="45" t="s">
+      <c r="V42" s="44"/>
+      <c r="W42" s="44"/>
+      <c r="X42" s="44"/>
+      <c r="Y42" s="44"/>
+      <c r="Z42" s="44"/>
+      <c r="AA42" s="44"/>
+      <c r="AB42" s="44"/>
+      <c r="AC42" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="AD42" s="45"/>
-      <c r="AE42" s="45"/>
-      <c r="AF42" s="45"/>
-      <c r="AG42" s="45"/>
-      <c r="AH42" s="45"/>
-      <c r="AI42" s="45"/>
-      <c r="AJ42" s="45"/>
+      <c r="AD42" s="44"/>
+      <c r="AE42" s="44"/>
+      <c r="AF42" s="44"/>
+      <c r="AG42" s="44"/>
+      <c r="AH42" s="44"/>
+      <c r="AI42" s="44"/>
+      <c r="AJ42" s="44"/>
       <c r="AK42" s="23"/>
       <c r="AL42" s="21"/>
       <c r="AM42" s="21"/>
@@ -10893,66 +10905,66 @@
       <c r="C48" t="s">
         <v>147</v>
       </c>
-      <c r="E48" s="45" t="s">
+      <c r="E48" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F48" s="45"/>
-      <c r="G48" s="45"/>
-      <c r="H48" s="45"/>
-      <c r="I48" s="45"/>
-      <c r="J48" s="45"/>
-      <c r="K48" s="45"/>
-      <c r="L48" s="45"/>
-      <c r="M48" s="45" t="s">
+      <c r="F48" s="44"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="44"/>
+      <c r="J48" s="44"/>
+      <c r="K48" s="44"/>
+      <c r="L48" s="44"/>
+      <c r="M48" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="N48" s="45"/>
-      <c r="O48" s="45"/>
-      <c r="P48" s="45"/>
-      <c r="Q48" s="45"/>
-      <c r="R48" s="45"/>
-      <c r="S48" s="45"/>
-      <c r="T48" s="45"/>
-      <c r="U48" s="45" t="s">
+      <c r="N48" s="44"/>
+      <c r="O48" s="44"/>
+      <c r="P48" s="44"/>
+      <c r="Q48" s="44"/>
+      <c r="R48" s="44"/>
+      <c r="S48" s="44"/>
+      <c r="T48" s="44"/>
+      <c r="U48" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="V48" s="45"/>
-      <c r="W48" s="45"/>
-      <c r="X48" s="45"/>
-      <c r="Y48" s="45"/>
-      <c r="Z48" s="45"/>
-      <c r="AA48" s="45"/>
-      <c r="AB48" s="45"/>
-      <c r="AC48" s="45" t="s">
+      <c r="V48" s="44"/>
+      <c r="W48" s="44"/>
+      <c r="X48" s="44"/>
+      <c r="Y48" s="44"/>
+      <c r="Z48" s="44"/>
+      <c r="AA48" s="44"/>
+      <c r="AB48" s="44"/>
+      <c r="AC48" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="AD48" s="45"/>
-      <c r="AE48" s="45"/>
-      <c r="AF48" s="45"/>
-      <c r="AG48" s="45"/>
-      <c r="AH48" s="45"/>
-      <c r="AI48" s="45"/>
-      <c r="AJ48" s="45"/>
-      <c r="AK48" s="45" t="s">
+      <c r="AD48" s="44"/>
+      <c r="AE48" s="44"/>
+      <c r="AF48" s="44"/>
+      <c r="AG48" s="44"/>
+      <c r="AH48" s="44"/>
+      <c r="AI48" s="44"/>
+      <c r="AJ48" s="44"/>
+      <c r="AK48" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="AL48" s="45"/>
-      <c r="AM48" s="45"/>
-      <c r="AN48" s="45"/>
-      <c r="AO48" s="45"/>
-      <c r="AP48" s="45"/>
-      <c r="AQ48" s="45"/>
-      <c r="AR48" s="45"/>
-      <c r="AS48" s="45" t="s">
+      <c r="AL48" s="44"/>
+      <c r="AM48" s="44"/>
+      <c r="AN48" s="44"/>
+      <c r="AO48" s="44"/>
+      <c r="AP48" s="44"/>
+      <c r="AQ48" s="44"/>
+      <c r="AR48" s="44"/>
+      <c r="AS48" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="AT48" s="45"/>
-      <c r="AU48" s="45"/>
-      <c r="AV48" s="45"/>
-      <c r="AW48" s="45"/>
-      <c r="AX48" s="45"/>
-      <c r="AY48" s="45"/>
-      <c r="AZ48" s="45"/>
+      <c r="AT48" s="44"/>
+      <c r="AU48" s="44"/>
+      <c r="AV48" s="44"/>
+      <c r="AW48" s="44"/>
+      <c r="AX48" s="44"/>
+      <c r="AY48" s="44"/>
+      <c r="AZ48" s="44"/>
       <c r="BA48" s="46"/>
       <c r="BB48" s="47"/>
       <c r="BC48" s="47"/>
@@ -11309,56 +11321,56 @@
       <c r="C54" t="s">
         <v>148</v>
       </c>
-      <c r="E54" s="45" t="s">
+      <c r="E54" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F54" s="45"/>
-      <c r="G54" s="45"/>
-      <c r="H54" s="45"/>
-      <c r="I54" s="45"/>
-      <c r="J54" s="45"/>
-      <c r="K54" s="45"/>
-      <c r="L54" s="45"/>
-      <c r="M54" s="45" t="s">
+      <c r="F54" s="44"/>
+      <c r="G54" s="44"/>
+      <c r="H54" s="44"/>
+      <c r="I54" s="44"/>
+      <c r="J54" s="44"/>
+      <c r="K54" s="44"/>
+      <c r="L54" s="44"/>
+      <c r="M54" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="N54" s="45"/>
-      <c r="O54" s="45"/>
-      <c r="P54" s="45"/>
-      <c r="Q54" s="45"/>
-      <c r="R54" s="45"/>
-      <c r="S54" s="45"/>
-      <c r="T54" s="45"/>
-      <c r="U54" s="45" t="s">
+      <c r="N54" s="44"/>
+      <c r="O54" s="44"/>
+      <c r="P54" s="44"/>
+      <c r="Q54" s="44"/>
+      <c r="R54" s="44"/>
+      <c r="S54" s="44"/>
+      <c r="T54" s="44"/>
+      <c r="U54" s="44" t="s">
         <v>180</v>
       </c>
-      <c r="V54" s="45"/>
-      <c r="W54" s="45"/>
-      <c r="X54" s="45"/>
-      <c r="Y54" s="45"/>
-      <c r="Z54" s="45"/>
-      <c r="AA54" s="45"/>
-      <c r="AB54" s="45"/>
-      <c r="AC54" s="45" t="s">
+      <c r="V54" s="44"/>
+      <c r="W54" s="44"/>
+      <c r="X54" s="44"/>
+      <c r="Y54" s="44"/>
+      <c r="Z54" s="44"/>
+      <c r="AA54" s="44"/>
+      <c r="AB54" s="44"/>
+      <c r="AC54" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="AD54" s="45"/>
-      <c r="AE54" s="45"/>
-      <c r="AF54" s="45"/>
-      <c r="AG54" s="45"/>
-      <c r="AH54" s="45"/>
-      <c r="AI54" s="45"/>
-      <c r="AJ54" s="45"/>
-      <c r="AK54" s="45" t="s">
+      <c r="AD54" s="44"/>
+      <c r="AE54" s="44"/>
+      <c r="AF54" s="44"/>
+      <c r="AG54" s="44"/>
+      <c r="AH54" s="44"/>
+      <c r="AI54" s="44"/>
+      <c r="AJ54" s="44"/>
+      <c r="AK54" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="AL54" s="45"/>
-      <c r="AM54" s="45"/>
-      <c r="AN54" s="45"/>
-      <c r="AO54" s="45"/>
-      <c r="AP54" s="45"/>
-      <c r="AQ54" s="45"/>
-      <c r="AR54" s="45"/>
+      <c r="AL54" s="44"/>
+      <c r="AM54" s="44"/>
+      <c r="AN54" s="44"/>
+      <c r="AO54" s="44"/>
+      <c r="AP54" s="44"/>
+      <c r="AQ54" s="44"/>
+      <c r="AR54" s="44"/>
       <c r="AS54" s="23"/>
       <c r="AT54" s="21"/>
       <c r="AU54" s="21"/>
@@ -11723,46 +11735,46 @@
       <c r="C60" t="s">
         <v>149</v>
       </c>
-      <c r="E60" s="45" t="s">
+      <c r="E60" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F60" s="45"/>
-      <c r="G60" s="45"/>
-      <c r="H60" s="45"/>
-      <c r="I60" s="45"/>
-      <c r="J60" s="45"/>
-      <c r="K60" s="45"/>
-      <c r="L60" s="45"/>
-      <c r="M60" s="45" t="s">
+      <c r="F60" s="44"/>
+      <c r="G60" s="44"/>
+      <c r="H60" s="44"/>
+      <c r="I60" s="44"/>
+      <c r="J60" s="44"/>
+      <c r="K60" s="44"/>
+      <c r="L60" s="44"/>
+      <c r="M60" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="N60" s="45"/>
-      <c r="O60" s="45"/>
-      <c r="P60" s="45"/>
-      <c r="Q60" s="45"/>
-      <c r="R60" s="45"/>
-      <c r="S60" s="45"/>
-      <c r="T60" s="45"/>
-      <c r="U60" s="45" t="s">
+      <c r="N60" s="44"/>
+      <c r="O60" s="44"/>
+      <c r="P60" s="44"/>
+      <c r="Q60" s="44"/>
+      <c r="R60" s="44"/>
+      <c r="S60" s="44"/>
+      <c r="T60" s="44"/>
+      <c r="U60" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="V60" s="45"/>
-      <c r="W60" s="45"/>
-      <c r="X60" s="45"/>
-      <c r="Y60" s="45"/>
-      <c r="Z60" s="45"/>
-      <c r="AA60" s="45"/>
-      <c r="AB60" s="45"/>
-      <c r="AC60" s="45" t="s">
+      <c r="V60" s="44"/>
+      <c r="W60" s="44"/>
+      <c r="X60" s="44"/>
+      <c r="Y60" s="44"/>
+      <c r="Z60" s="44"/>
+      <c r="AA60" s="44"/>
+      <c r="AB60" s="44"/>
+      <c r="AC60" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="AD60" s="45"/>
-      <c r="AE60" s="45"/>
-      <c r="AF60" s="45"/>
-      <c r="AG60" s="45"/>
-      <c r="AH60" s="45"/>
-      <c r="AI60" s="45"/>
-      <c r="AJ60" s="45"/>
+      <c r="AD60" s="44"/>
+      <c r="AE60" s="44"/>
+      <c r="AF60" s="44"/>
+      <c r="AG60" s="44"/>
+      <c r="AH60" s="44"/>
+      <c r="AI60" s="44"/>
+      <c r="AJ60" s="44"/>
       <c r="AK60" s="23"/>
       <c r="AL60" s="21"/>
       <c r="AM60" s="21"/>
@@ -12119,66 +12131,66 @@
       <c r="C66" t="s">
         <v>150</v>
       </c>
-      <c r="E66" s="45" t="s">
+      <c r="E66" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F66" s="45"/>
-      <c r="G66" s="45"/>
-      <c r="H66" s="45"/>
-      <c r="I66" s="45"/>
-      <c r="J66" s="45"/>
-      <c r="K66" s="45"/>
-      <c r="L66" s="45"/>
-      <c r="M66" s="45" t="s">
+      <c r="F66" s="44"/>
+      <c r="G66" s="44"/>
+      <c r="H66" s="44"/>
+      <c r="I66" s="44"/>
+      <c r="J66" s="44"/>
+      <c r="K66" s="44"/>
+      <c r="L66" s="44"/>
+      <c r="M66" s="44" t="s">
         <v>186</v>
       </c>
-      <c r="N66" s="45"/>
-      <c r="O66" s="45"/>
-      <c r="P66" s="45"/>
-      <c r="Q66" s="45"/>
-      <c r="R66" s="45"/>
-      <c r="S66" s="45"/>
-      <c r="T66" s="45"/>
-      <c r="U66" s="45" t="s">
+      <c r="N66" s="44"/>
+      <c r="O66" s="44"/>
+      <c r="P66" s="44"/>
+      <c r="Q66" s="44"/>
+      <c r="R66" s="44"/>
+      <c r="S66" s="44"/>
+      <c r="T66" s="44"/>
+      <c r="U66" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="V66" s="45"/>
-      <c r="W66" s="45"/>
-      <c r="X66" s="45"/>
-      <c r="Y66" s="45"/>
-      <c r="Z66" s="45"/>
-      <c r="AA66" s="45"/>
-      <c r="AB66" s="45"/>
-      <c r="AC66" s="45" t="s">
+      <c r="V66" s="44"/>
+      <c r="W66" s="44"/>
+      <c r="X66" s="44"/>
+      <c r="Y66" s="44"/>
+      <c r="Z66" s="44"/>
+      <c r="AA66" s="44"/>
+      <c r="AB66" s="44"/>
+      <c r="AC66" s="44" t="s">
         <v>180</v>
       </c>
-      <c r="AD66" s="45"/>
-      <c r="AE66" s="45"/>
-      <c r="AF66" s="45"/>
-      <c r="AG66" s="45"/>
-      <c r="AH66" s="45"/>
-      <c r="AI66" s="45"/>
-      <c r="AJ66" s="45"/>
-      <c r="AK66" s="45" t="s">
+      <c r="AD66" s="44"/>
+      <c r="AE66" s="44"/>
+      <c r="AF66" s="44"/>
+      <c r="AG66" s="44"/>
+      <c r="AH66" s="44"/>
+      <c r="AI66" s="44"/>
+      <c r="AJ66" s="44"/>
+      <c r="AK66" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="AL66" s="45"/>
-      <c r="AM66" s="45"/>
-      <c r="AN66" s="45"/>
-      <c r="AO66" s="45"/>
-      <c r="AP66" s="45"/>
-      <c r="AQ66" s="45"/>
-      <c r="AR66" s="45"/>
-      <c r="AS66" s="45" t="s">
+      <c r="AL66" s="44"/>
+      <c r="AM66" s="44"/>
+      <c r="AN66" s="44"/>
+      <c r="AO66" s="44"/>
+      <c r="AP66" s="44"/>
+      <c r="AQ66" s="44"/>
+      <c r="AR66" s="44"/>
+      <c r="AS66" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="AT66" s="45"/>
-      <c r="AU66" s="45"/>
-      <c r="AV66" s="45"/>
-      <c r="AW66" s="45"/>
-      <c r="AX66" s="45"/>
-      <c r="AY66" s="45"/>
-      <c r="AZ66" s="45"/>
+      <c r="AT66" s="44"/>
+      <c r="AU66" s="44"/>
+      <c r="AV66" s="44"/>
+      <c r="AW66" s="44"/>
+      <c r="AX66" s="44"/>
+      <c r="AY66" s="44"/>
+      <c r="AZ66" s="44"/>
       <c r="BA66" s="46"/>
       <c r="BB66" s="47"/>
       <c r="BC66" s="47"/>
@@ -12542,36 +12554,36 @@
       <c r="C72" t="s">
         <v>145</v>
       </c>
-      <c r="E72" s="45" t="s">
+      <c r="E72" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F72" s="45"/>
-      <c r="G72" s="45"/>
-      <c r="H72" s="45"/>
-      <c r="I72" s="45"/>
-      <c r="J72" s="45"/>
-      <c r="K72" s="45"/>
-      <c r="L72" s="45"/>
-      <c r="M72" s="45" t="s">
+      <c r="F72" s="44"/>
+      <c r="G72" s="44"/>
+      <c r="H72" s="44"/>
+      <c r="I72" s="44"/>
+      <c r="J72" s="44"/>
+      <c r="K72" s="44"/>
+      <c r="L72" s="44"/>
+      <c r="M72" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="N72" s="45"/>
-      <c r="O72" s="45"/>
-      <c r="P72" s="45"/>
-      <c r="Q72" s="45"/>
-      <c r="R72" s="45"/>
-      <c r="S72" s="45"/>
-      <c r="T72" s="45"/>
-      <c r="U72" s="45" t="s">
+      <c r="N72" s="44"/>
+      <c r="O72" s="44"/>
+      <c r="P72" s="44"/>
+      <c r="Q72" s="44"/>
+      <c r="R72" s="44"/>
+      <c r="S72" s="44"/>
+      <c r="T72" s="44"/>
+      <c r="U72" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="V72" s="45"/>
-      <c r="W72" s="45"/>
-      <c r="X72" s="45"/>
-      <c r="Y72" s="45"/>
-      <c r="Z72" s="45"/>
-      <c r="AA72" s="45"/>
-      <c r="AB72" s="45"/>
+      <c r="V72" s="44"/>
+      <c r="W72" s="44"/>
+      <c r="X72" s="44"/>
+      <c r="Y72" s="44"/>
+      <c r="Z72" s="44"/>
+      <c r="AA72" s="44"/>
+      <c r="AB72" s="44"/>
       <c r="AC72" s="23"/>
       <c r="AD72" s="21"/>
       <c r="AE72" s="21"/>
@@ -12934,46 +12946,46 @@
       <c r="C78" t="s">
         <v>146</v>
       </c>
-      <c r="E78" s="45" t="s">
+      <c r="E78" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F78" s="45"/>
-      <c r="G78" s="45"/>
-      <c r="H78" s="45"/>
-      <c r="I78" s="45"/>
-      <c r="J78" s="45"/>
-      <c r="K78" s="45"/>
-      <c r="L78" s="45"/>
-      <c r="M78" s="45" t="s">
+      <c r="F78" s="44"/>
+      <c r="G78" s="44"/>
+      <c r="H78" s="44"/>
+      <c r="I78" s="44"/>
+      <c r="J78" s="44"/>
+      <c r="K78" s="44"/>
+      <c r="L78" s="44"/>
+      <c r="M78" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="N78" s="45"/>
-      <c r="O78" s="45"/>
-      <c r="P78" s="45"/>
-      <c r="Q78" s="45"/>
-      <c r="R78" s="45"/>
-      <c r="S78" s="45"/>
-      <c r="T78" s="45"/>
-      <c r="U78" s="45" t="s">
+      <c r="N78" s="44"/>
+      <c r="O78" s="44"/>
+      <c r="P78" s="44"/>
+      <c r="Q78" s="44"/>
+      <c r="R78" s="44"/>
+      <c r="S78" s="44"/>
+      <c r="T78" s="44"/>
+      <c r="U78" s="44" t="s">
         <v>177</v>
       </c>
-      <c r="V78" s="45"/>
-      <c r="W78" s="45"/>
-      <c r="X78" s="45"/>
-      <c r="Y78" s="45"/>
-      <c r="Z78" s="45"/>
-      <c r="AA78" s="45"/>
-      <c r="AB78" s="45"/>
-      <c r="AC78" s="45" t="s">
+      <c r="V78" s="44"/>
+      <c r="W78" s="44"/>
+      <c r="X78" s="44"/>
+      <c r="Y78" s="44"/>
+      <c r="Z78" s="44"/>
+      <c r="AA78" s="44"/>
+      <c r="AB78" s="44"/>
+      <c r="AC78" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="AD78" s="45"/>
-      <c r="AE78" s="45"/>
-      <c r="AF78" s="45"/>
-      <c r="AG78" s="45"/>
-      <c r="AH78" s="45"/>
-      <c r="AI78" s="45"/>
-      <c r="AJ78" s="45"/>
+      <c r="AD78" s="44"/>
+      <c r="AE78" s="44"/>
+      <c r="AF78" s="44"/>
+      <c r="AG78" s="44"/>
+      <c r="AH78" s="44"/>
+      <c r="AI78" s="44"/>
+      <c r="AJ78" s="44"/>
       <c r="AK78" s="23"/>
       <c r="AL78" s="21"/>
       <c r="AM78" s="21"/>
@@ -13338,66 +13350,66 @@
       <c r="C84" t="s">
         <v>147</v>
       </c>
-      <c r="E84" s="45" t="s">
+      <c r="E84" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F84" s="45"/>
-      <c r="G84" s="45"/>
-      <c r="H84" s="45"/>
-      <c r="I84" s="45"/>
-      <c r="J84" s="45"/>
-      <c r="K84" s="45"/>
-      <c r="L84" s="45"/>
-      <c r="M84" s="45" t="s">
+      <c r="F84" s="44"/>
+      <c r="G84" s="44"/>
+      <c r="H84" s="44"/>
+      <c r="I84" s="44"/>
+      <c r="J84" s="44"/>
+      <c r="K84" s="44"/>
+      <c r="L84" s="44"/>
+      <c r="M84" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="N84" s="45"/>
-      <c r="O84" s="45"/>
-      <c r="P84" s="45"/>
-      <c r="Q84" s="45"/>
-      <c r="R84" s="45"/>
-      <c r="S84" s="45"/>
-      <c r="T84" s="45"/>
-      <c r="U84" s="45" t="s">
+      <c r="N84" s="44"/>
+      <c r="O84" s="44"/>
+      <c r="P84" s="44"/>
+      <c r="Q84" s="44"/>
+      <c r="R84" s="44"/>
+      <c r="S84" s="44"/>
+      <c r="T84" s="44"/>
+      <c r="U84" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="V84" s="45"/>
-      <c r="W84" s="45"/>
-      <c r="X84" s="45"/>
-      <c r="Y84" s="45"/>
-      <c r="Z84" s="45"/>
-      <c r="AA84" s="45"/>
-      <c r="AB84" s="45"/>
-      <c r="AC84" s="45" t="s">
+      <c r="V84" s="44"/>
+      <c r="W84" s="44"/>
+      <c r="X84" s="44"/>
+      <c r="Y84" s="44"/>
+      <c r="Z84" s="44"/>
+      <c r="AA84" s="44"/>
+      <c r="AB84" s="44"/>
+      <c r="AC84" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="AD84" s="45"/>
-      <c r="AE84" s="45"/>
-      <c r="AF84" s="45"/>
-      <c r="AG84" s="45"/>
-      <c r="AH84" s="45"/>
-      <c r="AI84" s="45"/>
-      <c r="AJ84" s="45"/>
-      <c r="AK84" s="45" t="s">
+      <c r="AD84" s="44"/>
+      <c r="AE84" s="44"/>
+      <c r="AF84" s="44"/>
+      <c r="AG84" s="44"/>
+      <c r="AH84" s="44"/>
+      <c r="AI84" s="44"/>
+      <c r="AJ84" s="44"/>
+      <c r="AK84" s="44" t="s">
         <v>177</v>
       </c>
-      <c r="AL84" s="45"/>
-      <c r="AM84" s="45"/>
-      <c r="AN84" s="45"/>
-      <c r="AO84" s="45"/>
-      <c r="AP84" s="45"/>
-      <c r="AQ84" s="45"/>
-      <c r="AR84" s="45"/>
-      <c r="AS84" s="45" t="s">
+      <c r="AL84" s="44"/>
+      <c r="AM84" s="44"/>
+      <c r="AN84" s="44"/>
+      <c r="AO84" s="44"/>
+      <c r="AP84" s="44"/>
+      <c r="AQ84" s="44"/>
+      <c r="AR84" s="44"/>
+      <c r="AS84" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="AT84" s="45"/>
-      <c r="AU84" s="45"/>
-      <c r="AV84" s="45"/>
-      <c r="AW84" s="45"/>
-      <c r="AX84" s="45"/>
-      <c r="AY84" s="45"/>
-      <c r="AZ84" s="45"/>
+      <c r="AT84" s="44"/>
+      <c r="AU84" s="44"/>
+      <c r="AV84" s="44"/>
+      <c r="AW84" s="44"/>
+      <c r="AX84" s="44"/>
+      <c r="AY84" s="44"/>
+      <c r="AZ84" s="44"/>
       <c r="BA84" s="46"/>
       <c r="BB84" s="47"/>
       <c r="BC84" s="47"/>
@@ -13758,56 +13770,56 @@
       <c r="C90" t="s">
         <v>148</v>
       </c>
-      <c r="E90" s="45" t="s">
+      <c r="E90" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F90" s="45"/>
-      <c r="G90" s="45"/>
-      <c r="H90" s="45"/>
-      <c r="I90" s="45"/>
-      <c r="J90" s="45"/>
-      <c r="K90" s="45"/>
-      <c r="L90" s="45"/>
-      <c r="M90" s="45" t="s">
+      <c r="F90" s="44"/>
+      <c r="G90" s="44"/>
+      <c r="H90" s="44"/>
+      <c r="I90" s="44"/>
+      <c r="J90" s="44"/>
+      <c r="K90" s="44"/>
+      <c r="L90" s="44"/>
+      <c r="M90" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="N90" s="45"/>
-      <c r="O90" s="45"/>
-      <c r="P90" s="45"/>
-      <c r="Q90" s="45"/>
-      <c r="R90" s="45"/>
-      <c r="S90" s="45"/>
-      <c r="T90" s="45"/>
-      <c r="U90" s="45" t="s">
+      <c r="N90" s="44"/>
+      <c r="O90" s="44"/>
+      <c r="P90" s="44"/>
+      <c r="Q90" s="44"/>
+      <c r="R90" s="44"/>
+      <c r="S90" s="44"/>
+      <c r="T90" s="44"/>
+      <c r="U90" s="44" t="s">
         <v>180</v>
       </c>
-      <c r="V90" s="45"/>
-      <c r="W90" s="45"/>
-      <c r="X90" s="45"/>
-      <c r="Y90" s="45"/>
-      <c r="Z90" s="45"/>
-      <c r="AA90" s="45"/>
-      <c r="AB90" s="45"/>
-      <c r="AC90" s="45" t="s">
+      <c r="V90" s="44"/>
+      <c r="W90" s="44"/>
+      <c r="X90" s="44"/>
+      <c r="Y90" s="44"/>
+      <c r="Z90" s="44"/>
+      <c r="AA90" s="44"/>
+      <c r="AB90" s="44"/>
+      <c r="AC90" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="AD90" s="45"/>
-      <c r="AE90" s="45"/>
-      <c r="AF90" s="45"/>
-      <c r="AG90" s="45"/>
-      <c r="AH90" s="45"/>
-      <c r="AI90" s="45"/>
-      <c r="AJ90" s="45"/>
-      <c r="AK90" s="45" t="s">
+      <c r="AD90" s="44"/>
+      <c r="AE90" s="44"/>
+      <c r="AF90" s="44"/>
+      <c r="AG90" s="44"/>
+      <c r="AH90" s="44"/>
+      <c r="AI90" s="44"/>
+      <c r="AJ90" s="44"/>
+      <c r="AK90" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="AL90" s="45"/>
-      <c r="AM90" s="45"/>
-      <c r="AN90" s="45"/>
-      <c r="AO90" s="45"/>
-      <c r="AP90" s="45"/>
-      <c r="AQ90" s="45"/>
-      <c r="AR90" s="45"/>
+      <c r="AL90" s="44"/>
+      <c r="AM90" s="44"/>
+      <c r="AN90" s="44"/>
+      <c r="AO90" s="44"/>
+      <c r="AP90" s="44"/>
+      <c r="AQ90" s="44"/>
+      <c r="AR90" s="44"/>
       <c r="AS90" s="23"/>
       <c r="AT90" s="21"/>
       <c r="AU90" s="21"/>
@@ -14176,46 +14188,46 @@
       <c r="C96" t="s">
         <v>149</v>
       </c>
-      <c r="E96" s="45" t="s">
+      <c r="E96" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F96" s="45"/>
-      <c r="G96" s="45"/>
-      <c r="H96" s="45"/>
-      <c r="I96" s="45"/>
-      <c r="J96" s="45"/>
-      <c r="K96" s="45"/>
-      <c r="L96" s="45"/>
-      <c r="M96" s="45" t="s">
+      <c r="F96" s="44"/>
+      <c r="G96" s="44"/>
+      <c r="H96" s="44"/>
+      <c r="I96" s="44"/>
+      <c r="J96" s="44"/>
+      <c r="K96" s="44"/>
+      <c r="L96" s="44"/>
+      <c r="M96" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="N96" s="45"/>
-      <c r="O96" s="45"/>
-      <c r="P96" s="45"/>
-      <c r="Q96" s="45"/>
-      <c r="R96" s="45"/>
-      <c r="S96" s="45"/>
-      <c r="T96" s="45"/>
-      <c r="U96" s="45" t="s">
+      <c r="N96" s="44"/>
+      <c r="O96" s="44"/>
+      <c r="P96" s="44"/>
+      <c r="Q96" s="44"/>
+      <c r="R96" s="44"/>
+      <c r="S96" s="44"/>
+      <c r="T96" s="44"/>
+      <c r="U96" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="V96" s="45"/>
-      <c r="W96" s="45"/>
-      <c r="X96" s="45"/>
-      <c r="Y96" s="45"/>
-      <c r="Z96" s="45"/>
-      <c r="AA96" s="45"/>
-      <c r="AB96" s="45"/>
-      <c r="AC96" s="45" t="s">
+      <c r="V96" s="44"/>
+      <c r="W96" s="44"/>
+      <c r="X96" s="44"/>
+      <c r="Y96" s="44"/>
+      <c r="Z96" s="44"/>
+      <c r="AA96" s="44"/>
+      <c r="AB96" s="44"/>
+      <c r="AC96" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="AD96" s="45"/>
-      <c r="AE96" s="45"/>
-      <c r="AF96" s="45"/>
-      <c r="AG96" s="45"/>
-      <c r="AH96" s="45"/>
-      <c r="AI96" s="45"/>
-      <c r="AJ96" s="45"/>
+      <c r="AD96" s="44"/>
+      <c r="AE96" s="44"/>
+      <c r="AF96" s="44"/>
+      <c r="AG96" s="44"/>
+      <c r="AH96" s="44"/>
+      <c r="AI96" s="44"/>
+      <c r="AJ96" s="44"/>
       <c r="AK96" s="23"/>
       <c r="AL96" s="21"/>
       <c r="AM96" s="21"/>
@@ -14576,66 +14588,66 @@
       <c r="C102" t="s">
         <v>150</v>
       </c>
-      <c r="E102" s="45" t="s">
+      <c r="E102" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F102" s="45"/>
-      <c r="G102" s="45"/>
-      <c r="H102" s="45"/>
-      <c r="I102" s="45"/>
-      <c r="J102" s="45"/>
-      <c r="K102" s="45"/>
-      <c r="L102" s="45"/>
-      <c r="M102" s="45" t="s">
+      <c r="F102" s="44"/>
+      <c r="G102" s="44"/>
+      <c r="H102" s="44"/>
+      <c r="I102" s="44"/>
+      <c r="J102" s="44"/>
+      <c r="K102" s="44"/>
+      <c r="L102" s="44"/>
+      <c r="M102" s="44" t="s">
         <v>186</v>
       </c>
-      <c r="N102" s="45"/>
-      <c r="O102" s="45"/>
-      <c r="P102" s="45"/>
-      <c r="Q102" s="45"/>
-      <c r="R102" s="45"/>
-      <c r="S102" s="45"/>
-      <c r="T102" s="45"/>
-      <c r="U102" s="45" t="s">
+      <c r="N102" s="44"/>
+      <c r="O102" s="44"/>
+      <c r="P102" s="44"/>
+      <c r="Q102" s="44"/>
+      <c r="R102" s="44"/>
+      <c r="S102" s="44"/>
+      <c r="T102" s="44"/>
+      <c r="U102" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="V102" s="45"/>
-      <c r="W102" s="45"/>
-      <c r="X102" s="45"/>
-      <c r="Y102" s="45"/>
-      <c r="Z102" s="45"/>
-      <c r="AA102" s="45"/>
-      <c r="AB102" s="45"/>
-      <c r="AC102" s="45" t="s">
+      <c r="V102" s="44"/>
+      <c r="W102" s="44"/>
+      <c r="X102" s="44"/>
+      <c r="Y102" s="44"/>
+      <c r="Z102" s="44"/>
+      <c r="AA102" s="44"/>
+      <c r="AB102" s="44"/>
+      <c r="AC102" s="44" t="s">
         <v>180</v>
       </c>
-      <c r="AD102" s="45"/>
-      <c r="AE102" s="45"/>
-      <c r="AF102" s="45"/>
-      <c r="AG102" s="45"/>
-      <c r="AH102" s="45"/>
-      <c r="AI102" s="45"/>
-      <c r="AJ102" s="45"/>
-      <c r="AK102" s="45" t="s">
+      <c r="AD102" s="44"/>
+      <c r="AE102" s="44"/>
+      <c r="AF102" s="44"/>
+      <c r="AG102" s="44"/>
+      <c r="AH102" s="44"/>
+      <c r="AI102" s="44"/>
+      <c r="AJ102" s="44"/>
+      <c r="AK102" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="AL102" s="45"/>
-      <c r="AM102" s="45"/>
-      <c r="AN102" s="45"/>
-      <c r="AO102" s="45"/>
-      <c r="AP102" s="45"/>
-      <c r="AQ102" s="45"/>
-      <c r="AR102" s="45"/>
-      <c r="AS102" s="45" t="s">
+      <c r="AL102" s="44"/>
+      <c r="AM102" s="44"/>
+      <c r="AN102" s="44"/>
+      <c r="AO102" s="44"/>
+      <c r="AP102" s="44"/>
+      <c r="AQ102" s="44"/>
+      <c r="AR102" s="44"/>
+      <c r="AS102" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="AT102" s="45"/>
-      <c r="AU102" s="45"/>
-      <c r="AV102" s="45"/>
-      <c r="AW102" s="45"/>
-      <c r="AX102" s="45"/>
-      <c r="AY102" s="45"/>
-      <c r="AZ102" s="45"/>
+      <c r="AT102" s="44"/>
+      <c r="AU102" s="44"/>
+      <c r="AV102" s="44"/>
+      <c r="AW102" s="44"/>
+      <c r="AX102" s="44"/>
+      <c r="AY102" s="44"/>
+      <c r="AZ102" s="44"/>
       <c r="BA102" s="46"/>
       <c r="BB102" s="47"/>
       <c r="BC102" s="47"/>
@@ -15003,56 +15015,56 @@
       <c r="C108" t="s">
         <v>145</v>
       </c>
-      <c r="E108" s="45" t="s">
+      <c r="E108" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F108" s="45"/>
-      <c r="G108" s="45"/>
-      <c r="H108" s="45"/>
-      <c r="I108" s="45"/>
-      <c r="J108" s="45"/>
-      <c r="K108" s="45"/>
-      <c r="L108" s="45"/>
-      <c r="M108" s="45" t="s">
+      <c r="F108" s="44"/>
+      <c r="G108" s="44"/>
+      <c r="H108" s="44"/>
+      <c r="I108" s="44"/>
+      <c r="J108" s="44"/>
+      <c r="K108" s="44"/>
+      <c r="L108" s="44"/>
+      <c r="M108" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="N108" s="45"/>
-      <c r="O108" s="45"/>
-      <c r="P108" s="45"/>
-      <c r="Q108" s="45"/>
-      <c r="R108" s="45"/>
-      <c r="S108" s="45"/>
-      <c r="T108" s="45"/>
-      <c r="U108" s="45" t="s">
+      <c r="N108" s="44"/>
+      <c r="O108" s="44"/>
+      <c r="P108" s="44"/>
+      <c r="Q108" s="44"/>
+      <c r="R108" s="44"/>
+      <c r="S108" s="44"/>
+      <c r="T108" s="44"/>
+      <c r="U108" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="V108" s="45"/>
-      <c r="W108" s="45"/>
-      <c r="X108" s="45"/>
-      <c r="Y108" s="45"/>
-      <c r="Z108" s="45"/>
-      <c r="AA108" s="45"/>
-      <c r="AB108" s="45"/>
-      <c r="AC108" s="45" t="s">
+      <c r="V108" s="44"/>
+      <c r="W108" s="44"/>
+      <c r="X108" s="44"/>
+      <c r="Y108" s="44"/>
+      <c r="Z108" s="44"/>
+      <c r="AA108" s="44"/>
+      <c r="AB108" s="44"/>
+      <c r="AC108" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="AD108" s="45"/>
-      <c r="AE108" s="45"/>
-      <c r="AF108" s="45"/>
-      <c r="AG108" s="45"/>
-      <c r="AH108" s="45"/>
-      <c r="AI108" s="45"/>
-      <c r="AJ108" s="45"/>
-      <c r="AK108" s="45" t="s">
+      <c r="AD108" s="44"/>
+      <c r="AE108" s="44"/>
+      <c r="AF108" s="44"/>
+      <c r="AG108" s="44"/>
+      <c r="AH108" s="44"/>
+      <c r="AI108" s="44"/>
+      <c r="AJ108" s="44"/>
+      <c r="AK108" s="44" t="s">
         <v>189</v>
       </c>
-      <c r="AL108" s="45"/>
-      <c r="AM108" s="45"/>
-      <c r="AN108" s="45"/>
-      <c r="AO108" s="45"/>
-      <c r="AP108" s="45"/>
-      <c r="AQ108" s="45"/>
-      <c r="AR108" s="45"/>
+      <c r="AL108" s="44"/>
+      <c r="AM108" s="44"/>
+      <c r="AN108" s="44"/>
+      <c r="AO108" s="44"/>
+      <c r="AP108" s="44"/>
+      <c r="AQ108" s="44"/>
+      <c r="AR108" s="44"/>
       <c r="AS108" s="23"/>
       <c r="AT108" s="21"/>
       <c r="AU108" s="21"/>
@@ -15424,66 +15436,66 @@
       <c r="C114" t="s">
         <v>146</v>
       </c>
-      <c r="E114" s="45" t="s">
+      <c r="E114" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F114" s="45"/>
-      <c r="G114" s="45"/>
-      <c r="H114" s="45"/>
-      <c r="I114" s="45"/>
-      <c r="J114" s="45"/>
-      <c r="K114" s="45"/>
-      <c r="L114" s="45"/>
-      <c r="M114" s="45" t="s">
+      <c r="F114" s="44"/>
+      <c r="G114" s="44"/>
+      <c r="H114" s="44"/>
+      <c r="I114" s="44"/>
+      <c r="J114" s="44"/>
+      <c r="K114" s="44"/>
+      <c r="L114" s="44"/>
+      <c r="M114" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="N114" s="45"/>
-      <c r="O114" s="45"/>
-      <c r="P114" s="45"/>
-      <c r="Q114" s="45"/>
-      <c r="R114" s="45"/>
-      <c r="S114" s="45"/>
-      <c r="T114" s="45"/>
-      <c r="U114" s="45" t="s">
+      <c r="N114" s="44"/>
+      <c r="O114" s="44"/>
+      <c r="P114" s="44"/>
+      <c r="Q114" s="44"/>
+      <c r="R114" s="44"/>
+      <c r="S114" s="44"/>
+      <c r="T114" s="44"/>
+      <c r="U114" s="44" t="s">
         <v>177</v>
       </c>
-      <c r="V114" s="45"/>
-      <c r="W114" s="45"/>
-      <c r="X114" s="45"/>
-      <c r="Y114" s="45"/>
-      <c r="Z114" s="45"/>
-      <c r="AA114" s="45"/>
-      <c r="AB114" s="45"/>
-      <c r="AC114" s="45" t="s">
+      <c r="V114" s="44"/>
+      <c r="W114" s="44"/>
+      <c r="X114" s="44"/>
+      <c r="Y114" s="44"/>
+      <c r="Z114" s="44"/>
+      <c r="AA114" s="44"/>
+      <c r="AB114" s="44"/>
+      <c r="AC114" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AD114" s="45"/>
-      <c r="AE114" s="45"/>
-      <c r="AF114" s="45"/>
-      <c r="AG114" s="45"/>
-      <c r="AH114" s="45"/>
-      <c r="AI114" s="45"/>
-      <c r="AJ114" s="45"/>
-      <c r="AK114" s="45" t="s">
+      <c r="AD114" s="44"/>
+      <c r="AE114" s="44"/>
+      <c r="AF114" s="44"/>
+      <c r="AG114" s="44"/>
+      <c r="AH114" s="44"/>
+      <c r="AI114" s="44"/>
+      <c r="AJ114" s="44"/>
+      <c r="AK114" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="AL114" s="45"/>
-      <c r="AM114" s="45"/>
-      <c r="AN114" s="45"/>
-      <c r="AO114" s="45"/>
-      <c r="AP114" s="45"/>
-      <c r="AQ114" s="45"/>
-      <c r="AR114" s="45"/>
-      <c r="AS114" s="45" t="s">
+      <c r="AL114" s="44"/>
+      <c r="AM114" s="44"/>
+      <c r="AN114" s="44"/>
+      <c r="AO114" s="44"/>
+      <c r="AP114" s="44"/>
+      <c r="AQ114" s="44"/>
+      <c r="AR114" s="44"/>
+      <c r="AS114" s="44" t="s">
         <v>189</v>
       </c>
-      <c r="AT114" s="45"/>
-      <c r="AU114" s="45"/>
-      <c r="AV114" s="45"/>
-      <c r="AW114" s="45"/>
-      <c r="AX114" s="45"/>
-      <c r="AY114" s="45"/>
-      <c r="AZ114" s="45"/>
+      <c r="AT114" s="44"/>
+      <c r="AU114" s="44"/>
+      <c r="AV114" s="44"/>
+      <c r="AW114" s="44"/>
+      <c r="AX114" s="44"/>
+      <c r="AY114" s="44"/>
+      <c r="AZ114" s="44"/>
       <c r="BA114" s="46"/>
       <c r="BB114" s="47"/>
       <c r="BC114" s="47"/>
@@ -15858,66 +15870,66 @@
       <c r="C120" t="s">
         <v>156</v>
       </c>
-      <c r="E120" s="45" t="s">
+      <c r="E120" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F120" s="45"/>
-      <c r="G120" s="45"/>
-      <c r="H120" s="45"/>
-      <c r="I120" s="45"/>
-      <c r="J120" s="45"/>
-      <c r="K120" s="45"/>
-      <c r="L120" s="45"/>
-      <c r="M120" s="45" t="s">
+      <c r="F120" s="44"/>
+      <c r="G120" s="44"/>
+      <c r="H120" s="44"/>
+      <c r="I120" s="44"/>
+      <c r="J120" s="44"/>
+      <c r="K120" s="44"/>
+      <c r="L120" s="44"/>
+      <c r="M120" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="N120" s="45"/>
-      <c r="O120" s="45"/>
-      <c r="P120" s="45"/>
-      <c r="Q120" s="45"/>
-      <c r="R120" s="45"/>
-      <c r="S120" s="45"/>
-      <c r="T120" s="45"/>
-      <c r="U120" s="45" t="s">
+      <c r="N120" s="44"/>
+      <c r="O120" s="44"/>
+      <c r="P120" s="44"/>
+      <c r="Q120" s="44"/>
+      <c r="R120" s="44"/>
+      <c r="S120" s="44"/>
+      <c r="T120" s="44"/>
+      <c r="U120" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="V120" s="45"/>
-      <c r="W120" s="45"/>
-      <c r="X120" s="45"/>
-      <c r="Y120" s="45"/>
-      <c r="Z120" s="45"/>
-      <c r="AA120" s="45"/>
-      <c r="AB120" s="45"/>
-      <c r="AC120" s="45" t="s">
+      <c r="V120" s="44"/>
+      <c r="W120" s="44"/>
+      <c r="X120" s="44"/>
+      <c r="Y120" s="44"/>
+      <c r="Z120" s="44"/>
+      <c r="AA120" s="44"/>
+      <c r="AB120" s="44"/>
+      <c r="AC120" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AD120" s="45"/>
-      <c r="AE120" s="45"/>
-      <c r="AF120" s="45"/>
-      <c r="AG120" s="45"/>
-      <c r="AH120" s="45"/>
-      <c r="AI120" s="45"/>
-      <c r="AJ120" s="45"/>
-      <c r="AK120" s="45" t="s">
+      <c r="AD120" s="44"/>
+      <c r="AE120" s="44"/>
+      <c r="AF120" s="44"/>
+      <c r="AG120" s="44"/>
+      <c r="AH120" s="44"/>
+      <c r="AI120" s="44"/>
+      <c r="AJ120" s="44"/>
+      <c r="AK120" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="AL120" s="45"/>
-      <c r="AM120" s="45"/>
-      <c r="AN120" s="45"/>
-      <c r="AO120" s="45"/>
-      <c r="AP120" s="45"/>
-      <c r="AQ120" s="45"/>
-      <c r="AR120" s="45"/>
-      <c r="AS120" s="45" t="s">
+      <c r="AL120" s="44"/>
+      <c r="AM120" s="44"/>
+      <c r="AN120" s="44"/>
+      <c r="AO120" s="44"/>
+      <c r="AP120" s="44"/>
+      <c r="AQ120" s="44"/>
+      <c r="AR120" s="44"/>
+      <c r="AS120" s="44" t="s">
         <v>189</v>
       </c>
-      <c r="AT120" s="45"/>
-      <c r="AU120" s="45"/>
-      <c r="AV120" s="45"/>
-      <c r="AW120" s="45"/>
-      <c r="AX120" s="45"/>
-      <c r="AY120" s="45"/>
-      <c r="AZ120" s="45"/>
+      <c r="AT120" s="44"/>
+      <c r="AU120" s="44"/>
+      <c r="AV120" s="44"/>
+      <c r="AW120" s="44"/>
+      <c r="AX120" s="44"/>
+      <c r="AY120" s="44"/>
+      <c r="AZ120" s="44"/>
       <c r="BA120" s="46"/>
       <c r="BB120" s="47"/>
       <c r="BC120" s="47"/>
@@ -16288,76 +16300,76 @@
       <c r="C126" t="s">
         <v>157</v>
       </c>
-      <c r="E126" s="45" t="s">
+      <c r="E126" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F126" s="45"/>
-      <c r="G126" s="45"/>
-      <c r="H126" s="45"/>
-      <c r="I126" s="45"/>
-      <c r="J126" s="45"/>
-      <c r="K126" s="45"/>
-      <c r="L126" s="45"/>
-      <c r="M126" s="45" t="s">
+      <c r="F126" s="44"/>
+      <c r="G126" s="44"/>
+      <c r="H126" s="44"/>
+      <c r="I126" s="44"/>
+      <c r="J126" s="44"/>
+      <c r="K126" s="44"/>
+      <c r="L126" s="44"/>
+      <c r="M126" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="N126" s="45"/>
-      <c r="O126" s="45"/>
-      <c r="P126" s="45"/>
-      <c r="Q126" s="45"/>
-      <c r="R126" s="45"/>
-      <c r="S126" s="45"/>
-      <c r="T126" s="45"/>
-      <c r="U126" s="45" t="s">
+      <c r="N126" s="44"/>
+      <c r="O126" s="44"/>
+      <c r="P126" s="44"/>
+      <c r="Q126" s="44"/>
+      <c r="R126" s="44"/>
+      <c r="S126" s="44"/>
+      <c r="T126" s="44"/>
+      <c r="U126" s="44" t="s">
         <v>180</v>
       </c>
-      <c r="V126" s="45"/>
-      <c r="W126" s="45"/>
-      <c r="X126" s="45"/>
-      <c r="Y126" s="45"/>
-      <c r="Z126" s="45"/>
-      <c r="AA126" s="45"/>
-      <c r="AB126" s="45"/>
-      <c r="AC126" s="45" t="s">
+      <c r="V126" s="44"/>
+      <c r="W126" s="44"/>
+      <c r="X126" s="44"/>
+      <c r="Y126" s="44"/>
+      <c r="Z126" s="44"/>
+      <c r="AA126" s="44"/>
+      <c r="AB126" s="44"/>
+      <c r="AC126" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="AD126" s="45"/>
-      <c r="AE126" s="45"/>
-      <c r="AF126" s="45"/>
-      <c r="AG126" s="45"/>
-      <c r="AH126" s="45"/>
-      <c r="AI126" s="45"/>
-      <c r="AJ126" s="45"/>
-      <c r="AK126" s="45" t="s">
+      <c r="AD126" s="44"/>
+      <c r="AE126" s="44"/>
+      <c r="AF126" s="44"/>
+      <c r="AG126" s="44"/>
+      <c r="AH126" s="44"/>
+      <c r="AI126" s="44"/>
+      <c r="AJ126" s="44"/>
+      <c r="AK126" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AL126" s="45"/>
-      <c r="AM126" s="45"/>
-      <c r="AN126" s="45"/>
-      <c r="AO126" s="45"/>
-      <c r="AP126" s="45"/>
-      <c r="AQ126" s="45"/>
-      <c r="AR126" s="45"/>
-      <c r="AS126" s="45" t="s">
+      <c r="AL126" s="44"/>
+      <c r="AM126" s="44"/>
+      <c r="AN126" s="44"/>
+      <c r="AO126" s="44"/>
+      <c r="AP126" s="44"/>
+      <c r="AQ126" s="44"/>
+      <c r="AR126" s="44"/>
+      <c r="AS126" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="AT126" s="45"/>
-      <c r="AU126" s="45"/>
-      <c r="AV126" s="45"/>
-      <c r="AW126" s="45"/>
-      <c r="AX126" s="45"/>
-      <c r="AY126" s="45"/>
-      <c r="AZ126" s="45"/>
-      <c r="BA126" s="45" t="s">
+      <c r="AT126" s="44"/>
+      <c r="AU126" s="44"/>
+      <c r="AV126" s="44"/>
+      <c r="AW126" s="44"/>
+      <c r="AX126" s="44"/>
+      <c r="AY126" s="44"/>
+      <c r="AZ126" s="44"/>
+      <c r="BA126" s="44" t="s">
         <v>189</v>
       </c>
-      <c r="BB126" s="45"/>
-      <c r="BC126" s="45"/>
-      <c r="BD126" s="45"/>
-      <c r="BE126" s="45"/>
-      <c r="BF126" s="45"/>
-      <c r="BG126" s="45"/>
-      <c r="BH126" s="45"/>
+      <c r="BB126" s="44"/>
+      <c r="BC126" s="44"/>
+      <c r="BD126" s="44"/>
+      <c r="BE126" s="44"/>
+      <c r="BF126" s="44"/>
+      <c r="BG126" s="44"/>
+      <c r="BH126" s="44"/>
     </row>
     <row r="127" spans="2:60">
       <c r="E127" s="29" t="s">
@@ -16741,36 +16753,36 @@
       <c r="C132" t="s">
         <v>160</v>
       </c>
-      <c r="E132" s="45" t="s">
+      <c r="E132" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F132" s="45"/>
-      <c r="G132" s="45"/>
-      <c r="H132" s="45"/>
-      <c r="I132" s="45"/>
-      <c r="J132" s="45"/>
-      <c r="K132" s="45"/>
-      <c r="L132" s="45"/>
-      <c r="M132" s="45" t="s">
+      <c r="F132" s="44"/>
+      <c r="G132" s="44"/>
+      <c r="H132" s="44"/>
+      <c r="I132" s="44"/>
+      <c r="J132" s="44"/>
+      <c r="K132" s="44"/>
+      <c r="L132" s="44"/>
+      <c r="M132" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="N132" s="45"/>
-      <c r="O132" s="45"/>
-      <c r="P132" s="45"/>
-      <c r="Q132" s="45"/>
-      <c r="R132" s="45"/>
-      <c r="S132" s="45"/>
-      <c r="T132" s="45"/>
-      <c r="U132" s="45" t="s">
+      <c r="N132" s="44"/>
+      <c r="O132" s="44"/>
+      <c r="P132" s="44"/>
+      <c r="Q132" s="44"/>
+      <c r="R132" s="44"/>
+      <c r="S132" s="44"/>
+      <c r="T132" s="44"/>
+      <c r="U132" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="V132" s="45"/>
-      <c r="W132" s="45"/>
-      <c r="X132" s="45"/>
-      <c r="Y132" s="45"/>
-      <c r="Z132" s="45"/>
-      <c r="AA132" s="45"/>
-      <c r="AB132" s="45"/>
+      <c r="V132" s="44"/>
+      <c r="W132" s="44"/>
+      <c r="X132" s="44"/>
+      <c r="Y132" s="44"/>
+      <c r="Z132" s="44"/>
+      <c r="AA132" s="44"/>
+      <c r="AB132" s="44"/>
       <c r="AC132" s="23"/>
       <c r="AD132" s="21"/>
       <c r="AE132" s="21"/>
@@ -17132,46 +17144,46 @@
       <c r="C138" t="s">
         <v>161</v>
       </c>
-      <c r="E138" s="45" t="s">
+      <c r="E138" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F138" s="45"/>
-      <c r="G138" s="45"/>
-      <c r="H138" s="45"/>
-      <c r="I138" s="45"/>
-      <c r="J138" s="45"/>
-      <c r="K138" s="45"/>
-      <c r="L138" s="45"/>
-      <c r="M138" s="45" t="s">
+      <c r="F138" s="44"/>
+      <c r="G138" s="44"/>
+      <c r="H138" s="44"/>
+      <c r="I138" s="44"/>
+      <c r="J138" s="44"/>
+      <c r="K138" s="44"/>
+      <c r="L138" s="44"/>
+      <c r="M138" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="N138" s="45"/>
-      <c r="O138" s="45"/>
-      <c r="P138" s="45"/>
-      <c r="Q138" s="45"/>
-      <c r="R138" s="45"/>
-      <c r="S138" s="45"/>
-      <c r="T138" s="45"/>
-      <c r="U138" s="45" t="s">
+      <c r="N138" s="44"/>
+      <c r="O138" s="44"/>
+      <c r="P138" s="44"/>
+      <c r="Q138" s="44"/>
+      <c r="R138" s="44"/>
+      <c r="S138" s="44"/>
+      <c r="T138" s="44"/>
+      <c r="U138" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="V138" s="45"/>
-      <c r="W138" s="45"/>
-      <c r="X138" s="45"/>
-      <c r="Y138" s="45"/>
-      <c r="Z138" s="45"/>
-      <c r="AA138" s="45"/>
-      <c r="AB138" s="45"/>
-      <c r="AC138" s="45" t="s">
+      <c r="V138" s="44"/>
+      <c r="W138" s="44"/>
+      <c r="X138" s="44"/>
+      <c r="Y138" s="44"/>
+      <c r="Z138" s="44"/>
+      <c r="AA138" s="44"/>
+      <c r="AB138" s="44"/>
+      <c r="AC138" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="AD138" s="45"/>
-      <c r="AE138" s="45"/>
-      <c r="AF138" s="45"/>
-      <c r="AG138" s="45"/>
-      <c r="AH138" s="45"/>
-      <c r="AI138" s="45"/>
-      <c r="AJ138" s="45"/>
+      <c r="AD138" s="44"/>
+      <c r="AE138" s="44"/>
+      <c r="AF138" s="44"/>
+      <c r="AG138" s="44"/>
+      <c r="AH138" s="44"/>
+      <c r="AI138" s="44"/>
+      <c r="AJ138" s="44"/>
       <c r="AK138" s="23"/>
       <c r="AL138" s="21"/>
       <c r="AM138" s="21"/>
@@ -17526,66 +17538,66 @@
       <c r="C144" t="s">
         <v>162</v>
       </c>
-      <c r="E144" s="45" t="s">
+      <c r="E144" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F144" s="45"/>
-      <c r="G144" s="45"/>
-      <c r="H144" s="45"/>
-      <c r="I144" s="45"/>
-      <c r="J144" s="45"/>
-      <c r="K144" s="45"/>
-      <c r="L144" s="45"/>
-      <c r="M144" s="45" t="s">
+      <c r="F144" s="44"/>
+      <c r="G144" s="44"/>
+      <c r="H144" s="44"/>
+      <c r="I144" s="44"/>
+      <c r="J144" s="44"/>
+      <c r="K144" s="44"/>
+      <c r="L144" s="44"/>
+      <c r="M144" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="N144" s="45"/>
-      <c r="O144" s="45"/>
-      <c r="P144" s="45"/>
-      <c r="Q144" s="45"/>
-      <c r="R144" s="45"/>
-      <c r="S144" s="45"/>
-      <c r="T144" s="45"/>
-      <c r="U144" s="45" t="s">
+      <c r="N144" s="44"/>
+      <c r="O144" s="44"/>
+      <c r="P144" s="44"/>
+      <c r="Q144" s="44"/>
+      <c r="R144" s="44"/>
+      <c r="S144" s="44"/>
+      <c r="T144" s="44"/>
+      <c r="U144" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="V144" s="45"/>
-      <c r="W144" s="45"/>
-      <c r="X144" s="45"/>
-      <c r="Y144" s="45"/>
-      <c r="Z144" s="45"/>
-      <c r="AA144" s="45"/>
-      <c r="AB144" s="45"/>
-      <c r="AC144" s="45" t="s">
+      <c r="V144" s="44"/>
+      <c r="W144" s="44"/>
+      <c r="X144" s="44"/>
+      <c r="Y144" s="44"/>
+      <c r="Z144" s="44"/>
+      <c r="AA144" s="44"/>
+      <c r="AB144" s="44"/>
+      <c r="AC144" s="44" t="s">
         <v>191</v>
       </c>
-      <c r="AD144" s="45"/>
-      <c r="AE144" s="45"/>
-      <c r="AF144" s="45"/>
-      <c r="AG144" s="45"/>
-      <c r="AH144" s="45"/>
-      <c r="AI144" s="45"/>
-      <c r="AJ144" s="45"/>
-      <c r="AK144" s="45" t="s">
+      <c r="AD144" s="44"/>
+      <c r="AE144" s="44"/>
+      <c r="AF144" s="44"/>
+      <c r="AG144" s="44"/>
+      <c r="AH144" s="44"/>
+      <c r="AI144" s="44"/>
+      <c r="AJ144" s="44"/>
+      <c r="AK144" s="44" t="s">
         <v>192</v>
       </c>
-      <c r="AL144" s="45"/>
-      <c r="AM144" s="45"/>
-      <c r="AN144" s="45"/>
-      <c r="AO144" s="45"/>
-      <c r="AP144" s="45"/>
-      <c r="AQ144" s="45"/>
-      <c r="AR144" s="45"/>
-      <c r="AS144" s="45" t="s">
+      <c r="AL144" s="44"/>
+      <c r="AM144" s="44"/>
+      <c r="AN144" s="44"/>
+      <c r="AO144" s="44"/>
+      <c r="AP144" s="44"/>
+      <c r="AQ144" s="44"/>
+      <c r="AR144" s="44"/>
+      <c r="AS144" s="44" t="s">
         <v>177</v>
       </c>
-      <c r="AT144" s="45"/>
-      <c r="AU144" s="45"/>
-      <c r="AV144" s="45"/>
-      <c r="AW144" s="45"/>
-      <c r="AX144" s="45"/>
-      <c r="AY144" s="45"/>
-      <c r="AZ144" s="45"/>
+      <c r="AT144" s="44"/>
+      <c r="AU144" s="44"/>
+      <c r="AV144" s="44"/>
+      <c r="AW144" s="44"/>
+      <c r="AX144" s="44"/>
+      <c r="AY144" s="44"/>
+      <c r="AZ144" s="44"/>
       <c r="BA144" s="31"/>
       <c r="BB144" s="21"/>
       <c r="BC144" s="21"/>
@@ -18312,66 +18324,66 @@
       <c r="C156" t="s">
         <v>164</v>
       </c>
-      <c r="E156" s="45" t="s">
+      <c r="E156" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F156" s="45"/>
-      <c r="G156" s="45"/>
-      <c r="H156" s="45"/>
-      <c r="I156" s="45"/>
-      <c r="J156" s="45"/>
-      <c r="K156" s="45"/>
-      <c r="L156" s="45"/>
-      <c r="M156" s="45" t="s">
+      <c r="F156" s="44"/>
+      <c r="G156" s="44"/>
+      <c r="H156" s="44"/>
+      <c r="I156" s="44"/>
+      <c r="J156" s="44"/>
+      <c r="K156" s="44"/>
+      <c r="L156" s="44"/>
+      <c r="M156" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="N156" s="45"/>
-      <c r="O156" s="45"/>
-      <c r="P156" s="45"/>
-      <c r="Q156" s="45"/>
-      <c r="R156" s="45"/>
-      <c r="S156" s="45"/>
-      <c r="T156" s="45"/>
-      <c r="U156" s="45" t="s">
+      <c r="N156" s="44"/>
+      <c r="O156" s="44"/>
+      <c r="P156" s="44"/>
+      <c r="Q156" s="44"/>
+      <c r="R156" s="44"/>
+      <c r="S156" s="44"/>
+      <c r="T156" s="44"/>
+      <c r="U156" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="V156" s="45"/>
-      <c r="W156" s="45"/>
-      <c r="X156" s="45"/>
-      <c r="Y156" s="45"/>
-      <c r="Z156" s="45"/>
-      <c r="AA156" s="45"/>
-      <c r="AB156" s="45"/>
-      <c r="AC156" s="45" t="s">
+      <c r="V156" s="44"/>
+      <c r="W156" s="44"/>
+      <c r="X156" s="44"/>
+      <c r="Y156" s="44"/>
+      <c r="Z156" s="44"/>
+      <c r="AA156" s="44"/>
+      <c r="AB156" s="44"/>
+      <c r="AC156" s="44" t="s">
         <v>193</v>
       </c>
-      <c r="AD156" s="45"/>
-      <c r="AE156" s="45"/>
-      <c r="AF156" s="45"/>
-      <c r="AG156" s="45"/>
-      <c r="AH156" s="45"/>
-      <c r="AI156" s="45"/>
-      <c r="AJ156" s="45"/>
-      <c r="AK156" s="45" t="s">
+      <c r="AD156" s="44"/>
+      <c r="AE156" s="44"/>
+      <c r="AF156" s="44"/>
+      <c r="AG156" s="44"/>
+      <c r="AH156" s="44"/>
+      <c r="AI156" s="44"/>
+      <c r="AJ156" s="44"/>
+      <c r="AK156" s="44" t="s">
         <v>194</v>
       </c>
-      <c r="AL156" s="45"/>
-      <c r="AM156" s="45"/>
-      <c r="AN156" s="45"/>
-      <c r="AO156" s="45"/>
-      <c r="AP156" s="45"/>
-      <c r="AQ156" s="45"/>
-      <c r="AR156" s="45"/>
-      <c r="AS156" s="45" t="s">
+      <c r="AL156" s="44"/>
+      <c r="AM156" s="44"/>
+      <c r="AN156" s="44"/>
+      <c r="AO156" s="44"/>
+      <c r="AP156" s="44"/>
+      <c r="AQ156" s="44"/>
+      <c r="AR156" s="44"/>
+      <c r="AS156" s="44" t="s">
         <v>195</v>
       </c>
-      <c r="AT156" s="45"/>
-      <c r="AU156" s="45"/>
-      <c r="AV156" s="45"/>
-      <c r="AW156" s="45"/>
-      <c r="AX156" s="45"/>
-      <c r="AY156" s="45"/>
-      <c r="AZ156" s="45"/>
+      <c r="AT156" s="44"/>
+      <c r="AU156" s="44"/>
+      <c r="AV156" s="44"/>
+      <c r="AW156" s="44"/>
+      <c r="AX156" s="44"/>
+      <c r="AY156" s="44"/>
+      <c r="AZ156" s="44"/>
       <c r="BA156" s="31"/>
       <c r="BB156" s="21"/>
       <c r="BC156" s="21"/>
@@ -18732,36 +18744,36 @@
       <c r="C162" t="s">
         <v>165</v>
       </c>
-      <c r="E162" s="45" t="s">
+      <c r="E162" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F162" s="45"/>
-      <c r="G162" s="45"/>
-      <c r="H162" s="45"/>
-      <c r="I162" s="45"/>
-      <c r="J162" s="45"/>
-      <c r="K162" s="45"/>
-      <c r="L162" s="45"/>
-      <c r="M162" s="45" t="s">
+      <c r="F162" s="44"/>
+      <c r="G162" s="44"/>
+      <c r="H162" s="44"/>
+      <c r="I162" s="44"/>
+      <c r="J162" s="44"/>
+      <c r="K162" s="44"/>
+      <c r="L162" s="44"/>
+      <c r="M162" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="N162" s="45"/>
-      <c r="O162" s="45"/>
-      <c r="P162" s="45"/>
-      <c r="Q162" s="45"/>
-      <c r="R162" s="45"/>
-      <c r="S162" s="45"/>
-      <c r="T162" s="45"/>
-      <c r="U162" s="45" t="s">
+      <c r="N162" s="44"/>
+      <c r="O162" s="44"/>
+      <c r="P162" s="44"/>
+      <c r="Q162" s="44"/>
+      <c r="R162" s="44"/>
+      <c r="S162" s="44"/>
+      <c r="T162" s="44"/>
+      <c r="U162" s="44" t="s">
         <v>177</v>
       </c>
-      <c r="V162" s="45"/>
-      <c r="W162" s="45"/>
-      <c r="X162" s="45"/>
-      <c r="Y162" s="45"/>
-      <c r="Z162" s="45"/>
-      <c r="AA162" s="45"/>
-      <c r="AB162" s="45"/>
+      <c r="V162" s="44"/>
+      <c r="W162" s="44"/>
+      <c r="X162" s="44"/>
+      <c r="Y162" s="44"/>
+      <c r="Z162" s="44"/>
+      <c r="AA162" s="44"/>
+      <c r="AB162" s="44"/>
       <c r="AC162" s="23"/>
       <c r="AD162" s="21"/>
       <c r="AE162" s="21"/>
@@ -19124,56 +19136,56 @@
       <c r="C168" t="s">
         <v>166</v>
       </c>
-      <c r="E168" s="45" t="s">
+      <c r="E168" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F168" s="45"/>
-      <c r="G168" s="45"/>
-      <c r="H168" s="45"/>
-      <c r="I168" s="45"/>
-      <c r="J168" s="45"/>
-      <c r="K168" s="45"/>
-      <c r="L168" s="45"/>
-      <c r="M168" s="45" t="s">
+      <c r="F168" s="44"/>
+      <c r="G168" s="44"/>
+      <c r="H168" s="44"/>
+      <c r="I168" s="44"/>
+      <c r="J168" s="44"/>
+      <c r="K168" s="44"/>
+      <c r="L168" s="44"/>
+      <c r="M168" s="44" t="s">
         <v>186</v>
       </c>
-      <c r="N168" s="45"/>
-      <c r="O168" s="45"/>
-      <c r="P168" s="45"/>
-      <c r="Q168" s="45"/>
-      <c r="R168" s="45"/>
-      <c r="S168" s="45"/>
-      <c r="T168" s="45"/>
-      <c r="U168" s="45" t="s">
+      <c r="N168" s="44"/>
+      <c r="O168" s="44"/>
+      <c r="P168" s="44"/>
+      <c r="Q168" s="44"/>
+      <c r="R168" s="44"/>
+      <c r="S168" s="44"/>
+      <c r="T168" s="44"/>
+      <c r="U168" s="44" t="s">
         <v>196</v>
       </c>
-      <c r="V168" s="45"/>
-      <c r="W168" s="45"/>
-      <c r="X168" s="45"/>
-      <c r="Y168" s="45"/>
-      <c r="Z168" s="45"/>
-      <c r="AA168" s="45"/>
-      <c r="AB168" s="45"/>
-      <c r="AC168" s="45" t="s">
+      <c r="V168" s="44"/>
+      <c r="W168" s="44"/>
+      <c r="X168" s="44"/>
+      <c r="Y168" s="44"/>
+      <c r="Z168" s="44"/>
+      <c r="AA168" s="44"/>
+      <c r="AB168" s="44"/>
+      <c r="AC168" s="44" t="s">
         <v>178</v>
       </c>
-      <c r="AD168" s="45"/>
-      <c r="AE168" s="45"/>
-      <c r="AF168" s="45"/>
-      <c r="AG168" s="45"/>
-      <c r="AH168" s="45"/>
-      <c r="AI168" s="45"/>
-      <c r="AJ168" s="45"/>
-      <c r="AK168" s="45" t="s">
+      <c r="AD168" s="44"/>
+      <c r="AE168" s="44"/>
+      <c r="AF168" s="44"/>
+      <c r="AG168" s="44"/>
+      <c r="AH168" s="44"/>
+      <c r="AI168" s="44"/>
+      <c r="AJ168" s="44"/>
+      <c r="AK168" s="44" t="s">
         <v>177</v>
       </c>
-      <c r="AL168" s="45"/>
-      <c r="AM168" s="45"/>
-      <c r="AN168" s="45"/>
-      <c r="AO168" s="45"/>
-      <c r="AP168" s="45"/>
-      <c r="AQ168" s="45"/>
-      <c r="AR168" s="45"/>
+      <c r="AL168" s="44"/>
+      <c r="AM168" s="44"/>
+      <c r="AN168" s="44"/>
+      <c r="AO168" s="44"/>
+      <c r="AP168" s="44"/>
+      <c r="AQ168" s="44"/>
+      <c r="AR168" s="44"/>
       <c r="AS168" s="23"/>
       <c r="AT168" s="21"/>
       <c r="AU168" s="21"/>
@@ -19534,66 +19546,66 @@
       <c r="C174" t="s">
         <v>167</v>
       </c>
-      <c r="E174" s="45" t="s">
+      <c r="E174" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F174" s="45"/>
-      <c r="G174" s="45"/>
-      <c r="H174" s="45"/>
-      <c r="I174" s="45"/>
-      <c r="J174" s="45"/>
-      <c r="K174" s="45"/>
-      <c r="L174" s="45"/>
-      <c r="M174" s="45" t="s">
+      <c r="F174" s="44"/>
+      <c r="G174" s="44"/>
+      <c r="H174" s="44"/>
+      <c r="I174" s="44"/>
+      <c r="J174" s="44"/>
+      <c r="K174" s="44"/>
+      <c r="L174" s="44"/>
+      <c r="M174" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="N174" s="45"/>
-      <c r="O174" s="45"/>
-      <c r="P174" s="45"/>
-      <c r="Q174" s="45"/>
-      <c r="R174" s="45"/>
-      <c r="S174" s="45"/>
-      <c r="T174" s="45"/>
-      <c r="U174" s="45" t="s">
+      <c r="N174" s="44"/>
+      <c r="O174" s="44"/>
+      <c r="P174" s="44"/>
+      <c r="Q174" s="44"/>
+      <c r="R174" s="44"/>
+      <c r="S174" s="44"/>
+      <c r="T174" s="44"/>
+      <c r="U174" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="V174" s="45"/>
-      <c r="W174" s="45"/>
-      <c r="X174" s="45"/>
-      <c r="Y174" s="45"/>
-      <c r="Z174" s="45"/>
-      <c r="AA174" s="45"/>
-      <c r="AB174" s="45"/>
-      <c r="AC174" s="45" t="s">
+      <c r="V174" s="44"/>
+      <c r="W174" s="44"/>
+      <c r="X174" s="44"/>
+      <c r="Y174" s="44"/>
+      <c r="Z174" s="44"/>
+      <c r="AA174" s="44"/>
+      <c r="AB174" s="44"/>
+      <c r="AC174" s="44" t="s">
         <v>194</v>
       </c>
-      <c r="AD174" s="45"/>
-      <c r="AE174" s="45"/>
-      <c r="AF174" s="45"/>
-      <c r="AG174" s="45"/>
-      <c r="AH174" s="45"/>
-      <c r="AI174" s="45"/>
-      <c r="AJ174" s="45"/>
-      <c r="AK174" s="45" t="s">
+      <c r="AD174" s="44"/>
+      <c r="AE174" s="44"/>
+      <c r="AF174" s="44"/>
+      <c r="AG174" s="44"/>
+      <c r="AH174" s="44"/>
+      <c r="AI174" s="44"/>
+      <c r="AJ174" s="44"/>
+      <c r="AK174" s="44" t="s">
         <v>195</v>
       </c>
-      <c r="AL174" s="45"/>
-      <c r="AM174" s="45"/>
-      <c r="AN174" s="45"/>
-      <c r="AO174" s="45"/>
-      <c r="AP174" s="45"/>
-      <c r="AQ174" s="45"/>
-      <c r="AR174" s="45"/>
-      <c r="AS174" s="45" t="s">
+      <c r="AL174" s="44"/>
+      <c r="AM174" s="44"/>
+      <c r="AN174" s="44"/>
+      <c r="AO174" s="44"/>
+      <c r="AP174" s="44"/>
+      <c r="AQ174" s="44"/>
+      <c r="AR174" s="44"/>
+      <c r="AS174" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="AT174" s="45"/>
-      <c r="AU174" s="45"/>
-      <c r="AV174" s="45"/>
-      <c r="AW174" s="45"/>
-      <c r="AX174" s="45"/>
-      <c r="AY174" s="45"/>
-      <c r="AZ174" s="45"/>
+      <c r="AT174" s="44"/>
+      <c r="AU174" s="44"/>
+      <c r="AV174" s="44"/>
+      <c r="AW174" s="44"/>
+      <c r="AX174" s="44"/>
+      <c r="AY174" s="44"/>
+      <c r="AZ174" s="44"/>
       <c r="BA174" s="31"/>
       <c r="BB174" s="21"/>
       <c r="BC174" s="21"/>
@@ -19950,46 +19962,46 @@
       <c r="C180" t="s">
         <v>168</v>
       </c>
-      <c r="E180" s="45" t="s">
+      <c r="E180" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="F180" s="45"/>
-      <c r="G180" s="45"/>
-      <c r="H180" s="45"/>
-      <c r="I180" s="45"/>
-      <c r="J180" s="45"/>
-      <c r="K180" s="45"/>
-      <c r="L180" s="45"/>
-      <c r="M180" s="45" t="s">
+      <c r="F180" s="44"/>
+      <c r="G180" s="44"/>
+      <c r="H180" s="44"/>
+      <c r="I180" s="44"/>
+      <c r="J180" s="44"/>
+      <c r="K180" s="44"/>
+      <c r="L180" s="44"/>
+      <c r="M180" s="44" t="s">
         <v>197</v>
       </c>
-      <c r="N180" s="45"/>
-      <c r="O180" s="45"/>
-      <c r="P180" s="45"/>
-      <c r="Q180" s="45"/>
-      <c r="R180" s="45"/>
-      <c r="S180" s="45"/>
-      <c r="T180" s="45"/>
-      <c r="U180" s="45" t="s">
+      <c r="N180" s="44"/>
+      <c r="O180" s="44"/>
+      <c r="P180" s="44"/>
+      <c r="Q180" s="44"/>
+      <c r="R180" s="44"/>
+      <c r="S180" s="44"/>
+      <c r="T180" s="44"/>
+      <c r="U180" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="V180" s="45"/>
-      <c r="W180" s="45"/>
-      <c r="X180" s="45"/>
-      <c r="Y180" s="45"/>
-      <c r="Z180" s="45"/>
-      <c r="AA180" s="45"/>
-      <c r="AB180" s="45"/>
-      <c r="AC180" s="45" t="s">
+      <c r="V180" s="44"/>
+      <c r="W180" s="44"/>
+      <c r="X180" s="44"/>
+      <c r="Y180" s="44"/>
+      <c r="Z180" s="44"/>
+      <c r="AA180" s="44"/>
+      <c r="AB180" s="44"/>
+      <c r="AC180" s="44" t="s">
         <v>199</v>
       </c>
-      <c r="AD180" s="45"/>
-      <c r="AE180" s="45"/>
-      <c r="AF180" s="45"/>
-      <c r="AG180" s="45"/>
-      <c r="AH180" s="45"/>
-      <c r="AI180" s="45"/>
-      <c r="AJ180" s="45"/>
+      <c r="AD180" s="44"/>
+      <c r="AE180" s="44"/>
+      <c r="AF180" s="44"/>
+      <c r="AG180" s="44"/>
+      <c r="AH180" s="44"/>
+      <c r="AI180" s="44"/>
+      <c r="AJ180" s="44"/>
       <c r="AK180" s="23"/>
       <c r="AL180" s="21"/>
       <c r="AM180" s="21"/>
@@ -20354,7 +20366,7 @@
       <c r="F192" s="42"/>
       <c r="G192" s="42"/>
       <c r="H192" s="43"/>
-      <c r="I192" s="44" t="s">
+      <c r="I192" s="45" t="s">
         <v>243</v>
       </c>
       <c r="J192" s="42"/>
@@ -20943,13 +20955,25 @@
       <c r="K238" s="15"/>
       <c r="L238" s="16"/>
     </row>
-    <row r="241" spans="2:8" s="20" customFormat="1"/>
-    <row r="243" spans="2:8">
+    <row r="241" spans="2:12" s="20" customFormat="1"/>
+    <row r="243" spans="2:12">
       <c r="B243" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="244" spans="2:8">
+      <c r="E243" s="44" t="s">
+        <v>276</v>
+      </c>
+      <c r="F243" s="44"/>
+      <c r="G243" s="44"/>
+      <c r="H243" s="44"/>
+      <c r="I243" s="44" t="s">
+        <v>277</v>
+      </c>
+      <c r="J243" s="44"/>
+      <c r="K243" s="44"/>
+      <c r="L243" s="44"/>
+    </row>
+    <row r="244" spans="2:12">
       <c r="C244" t="s">
         <v>270</v>
       </c>
@@ -20959,8 +20983,14 @@
       <c r="F244" s="42"/>
       <c r="G244" s="42"/>
       <c r="H244" s="43"/>
-    </row>
-    <row r="245" spans="2:8">
+      <c r="I244" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="J244" s="42"/>
+      <c r="K244" s="42"/>
+      <c r="L244" s="43"/>
+    </row>
+    <row r="245" spans="2:12">
       <c r="E245" s="14" t="str">
         <f>E244&amp;"0"</f>
         <v>AD_SET0</v>
@@ -20977,8 +21007,24 @@
         <f>E244&amp;"3"</f>
         <v>AD_SET3</v>
       </c>
-    </row>
-    <row r="246" spans="2:8">
+      <c r="I245" s="14" t="str">
+        <f>I244&amp;"0"</f>
+        <v>REG_SET0</v>
+      </c>
+      <c r="J245" s="14" t="str">
+        <f>I244&amp;"1"</f>
+        <v>REG_SET1</v>
+      </c>
+      <c r="K245" s="14" t="str">
+        <f>I244&amp;"2"</f>
+        <v>REG_SET2</v>
+      </c>
+      <c r="L245" s="10" t="str">
+        <f>I244&amp;"3"</f>
+        <v>REG_SET3</v>
+      </c>
+    </row>
+    <row r="246" spans="2:12">
       <c r="E246" s="17" t="s">
         <v>271</v>
       </c>
@@ -20987,73 +21033,142 @@
       </c>
       <c r="G246" s="18"/>
       <c r="H246" s="19"/>
-    </row>
-    <row r="247" spans="2:8">
-      <c r="E247" s="14"/>
-      <c r="F247" s="15" t="s">
-        <v>274</v>
-      </c>
-      <c r="G247" s="15"/>
-      <c r="H247" s="16"/>
-    </row>
-    <row r="249" spans="2:8">
-      <c r="E249" s="41" t="s">
+      <c r="I246" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="F249" s="42"/>
-      <c r="G249" s="42"/>
-      <c r="H249" s="43"/>
-    </row>
-    <row r="250" spans="2:8">
-      <c r="E250" s="14" t="str">
-        <f>E249&amp;"0"</f>
-        <v>REG_SET0</v>
-      </c>
-      <c r="F250" s="14" t="str">
-        <f>E249&amp;"1"</f>
-        <v>REG_SET1</v>
-      </c>
-      <c r="G250" s="14" t="str">
-        <f>E249&amp;"2"</f>
-        <v>REG_SET2</v>
-      </c>
-      <c r="H250" s="10" t="str">
-        <f>E249&amp;"3"</f>
-        <v>REG_SET3</v>
-      </c>
-    </row>
-    <row r="251" spans="2:8">
-      <c r="E251" s="17" t="s">
-        <v>276</v>
-      </c>
-      <c r="F251" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="G251" s="18"/>
-      <c r="H251" s="19"/>
-    </row>
-    <row r="252" spans="2:8">
-      <c r="E252" s="14"/>
-      <c r="F252" s="15"/>
-      <c r="G252" s="15"/>
-      <c r="H252" s="16"/>
+      <c r="J246" s="18"/>
+      <c r="K246" s="18"/>
+      <c r="L246" s="19"/>
+    </row>
+    <row r="247" spans="2:12">
+      <c r="E247" s="13"/>
+      <c r="F247" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="G247" s="11"/>
+      <c r="H247" s="12"/>
+      <c r="I247" s="13"/>
+      <c r="J247" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="K247" s="11"/>
+      <c r="L247" s="12"/>
+    </row>
+    <row r="248" spans="2:12">
+      <c r="E248" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="F248" s="15"/>
+      <c r="G248" s="15"/>
+      <c r="H248" s="16"/>
+      <c r="I248" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="J248" s="15"/>
+      <c r="K248" s="15"/>
+      <c r="L248" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="138">
-    <mergeCell ref="E244:H244"/>
-    <mergeCell ref="E249:H249"/>
-    <mergeCell ref="E162:L162"/>
-    <mergeCell ref="E168:L168"/>
-    <mergeCell ref="E174:L174"/>
-    <mergeCell ref="E180:L180"/>
-    <mergeCell ref="E192:H192"/>
-    <mergeCell ref="I192:L192"/>
-    <mergeCell ref="E108:L108"/>
-    <mergeCell ref="E114:L114"/>
-    <mergeCell ref="E120:L120"/>
-    <mergeCell ref="E126:L126"/>
-    <mergeCell ref="E132:L132"/>
-    <mergeCell ref="E138:L138"/>
+  <mergeCells count="140">
+    <mergeCell ref="AK120:AR120"/>
+    <mergeCell ref="AK126:AR126"/>
+    <mergeCell ref="AK144:AR144"/>
+    <mergeCell ref="E24:L24"/>
+    <mergeCell ref="M24:T24"/>
+    <mergeCell ref="E30:L30"/>
+    <mergeCell ref="M30:T30"/>
+    <mergeCell ref="M36:T36"/>
+    <mergeCell ref="BA21:BH21"/>
+    <mergeCell ref="AC42:AJ42"/>
+    <mergeCell ref="E21:L21"/>
+    <mergeCell ref="M21:T21"/>
+    <mergeCell ref="U21:AB21"/>
+    <mergeCell ref="AC21:AJ21"/>
+    <mergeCell ref="AK21:AR21"/>
+    <mergeCell ref="M84:T84"/>
+    <mergeCell ref="E144:L144"/>
+    <mergeCell ref="BA48:BD48"/>
+    <mergeCell ref="BA66:BD66"/>
+    <mergeCell ref="BA84:BD84"/>
+    <mergeCell ref="BA102:BD102"/>
+    <mergeCell ref="BA114:BD114"/>
+    <mergeCell ref="BA120:BD120"/>
+    <mergeCell ref="M42:T42"/>
+    <mergeCell ref="E84:L84"/>
+    <mergeCell ref="E90:L90"/>
+    <mergeCell ref="E96:L96"/>
+    <mergeCell ref="E102:L102"/>
+    <mergeCell ref="E78:L78"/>
+    <mergeCell ref="AS21:AZ21"/>
+    <mergeCell ref="AC96:AJ96"/>
+    <mergeCell ref="AC102:AJ102"/>
+    <mergeCell ref="AC108:AJ108"/>
+    <mergeCell ref="U108:AB108"/>
+    <mergeCell ref="M48:T48"/>
+    <mergeCell ref="M54:T54"/>
+    <mergeCell ref="M60:T60"/>
+    <mergeCell ref="M162:T162"/>
+    <mergeCell ref="M168:T168"/>
+    <mergeCell ref="M174:T174"/>
+    <mergeCell ref="M180:T180"/>
+    <mergeCell ref="U36:AB36"/>
+    <mergeCell ref="U42:AB42"/>
+    <mergeCell ref="U48:AB48"/>
+    <mergeCell ref="U54:AB54"/>
+    <mergeCell ref="U60:AB60"/>
+    <mergeCell ref="U66:AB66"/>
+    <mergeCell ref="M90:T90"/>
+    <mergeCell ref="M96:T96"/>
+    <mergeCell ref="M102:T102"/>
+    <mergeCell ref="M108:T108"/>
+    <mergeCell ref="M114:T114"/>
+    <mergeCell ref="M120:T120"/>
+    <mergeCell ref="M132:T132"/>
+    <mergeCell ref="M138:T138"/>
+    <mergeCell ref="M144:T144"/>
+    <mergeCell ref="M156:T156"/>
+    <mergeCell ref="M126:T126"/>
+    <mergeCell ref="M66:T66"/>
+    <mergeCell ref="M72:T72"/>
+    <mergeCell ref="M78:T78"/>
+    <mergeCell ref="U168:AB168"/>
+    <mergeCell ref="U174:AB174"/>
+    <mergeCell ref="U180:AB180"/>
+    <mergeCell ref="U72:AB72"/>
+    <mergeCell ref="U78:AB78"/>
+    <mergeCell ref="U84:AB84"/>
+    <mergeCell ref="U90:AB90"/>
+    <mergeCell ref="U96:AB96"/>
+    <mergeCell ref="U102:AB102"/>
+    <mergeCell ref="U120:AB120"/>
+    <mergeCell ref="U126:AB126"/>
+    <mergeCell ref="U132:AB132"/>
+    <mergeCell ref="U138:AB138"/>
+    <mergeCell ref="U114:AB114"/>
+    <mergeCell ref="AC180:AJ180"/>
+    <mergeCell ref="AK48:AR48"/>
+    <mergeCell ref="AK54:AR54"/>
+    <mergeCell ref="AK66:AR66"/>
+    <mergeCell ref="AK84:AR84"/>
+    <mergeCell ref="AK90:AR90"/>
+    <mergeCell ref="AK102:AR102"/>
+    <mergeCell ref="AK108:AR108"/>
+    <mergeCell ref="AK114:AR114"/>
+    <mergeCell ref="AC114:AJ114"/>
+    <mergeCell ref="AC120:AJ120"/>
+    <mergeCell ref="AC126:AJ126"/>
+    <mergeCell ref="AC138:AJ138"/>
+    <mergeCell ref="AC144:AJ144"/>
+    <mergeCell ref="AC156:AJ156"/>
+    <mergeCell ref="AC48:AJ48"/>
+    <mergeCell ref="AC54:AJ54"/>
+    <mergeCell ref="AC60:AJ60"/>
+    <mergeCell ref="AC66:AJ66"/>
+    <mergeCell ref="AC78:AJ78"/>
+    <mergeCell ref="AC84:AJ84"/>
+    <mergeCell ref="AK156:AR156"/>
+    <mergeCell ref="AC168:AJ168"/>
+    <mergeCell ref="AC90:AJ90"/>
     <mergeCell ref="AS156:AZ156"/>
     <mergeCell ref="AS174:AZ174"/>
     <mergeCell ref="BA126:BH126"/>
@@ -21078,106 +21193,23 @@
     <mergeCell ref="U144:AB144"/>
     <mergeCell ref="U156:AB156"/>
     <mergeCell ref="U162:AB162"/>
-    <mergeCell ref="AC180:AJ180"/>
-    <mergeCell ref="AK48:AR48"/>
-    <mergeCell ref="AK54:AR54"/>
-    <mergeCell ref="AK66:AR66"/>
-    <mergeCell ref="AK84:AR84"/>
-    <mergeCell ref="AK90:AR90"/>
-    <mergeCell ref="AK102:AR102"/>
-    <mergeCell ref="AK108:AR108"/>
-    <mergeCell ref="AK114:AR114"/>
-    <mergeCell ref="AC114:AJ114"/>
-    <mergeCell ref="AC120:AJ120"/>
-    <mergeCell ref="AC126:AJ126"/>
-    <mergeCell ref="AC138:AJ138"/>
-    <mergeCell ref="AC144:AJ144"/>
-    <mergeCell ref="AC156:AJ156"/>
-    <mergeCell ref="AC48:AJ48"/>
-    <mergeCell ref="AC54:AJ54"/>
-    <mergeCell ref="AC60:AJ60"/>
-    <mergeCell ref="AC66:AJ66"/>
-    <mergeCell ref="AC78:AJ78"/>
-    <mergeCell ref="AC84:AJ84"/>
-    <mergeCell ref="AK156:AR156"/>
-    <mergeCell ref="AC168:AJ168"/>
-    <mergeCell ref="AC90:AJ90"/>
-    <mergeCell ref="U168:AB168"/>
-    <mergeCell ref="U174:AB174"/>
-    <mergeCell ref="U180:AB180"/>
-    <mergeCell ref="U72:AB72"/>
-    <mergeCell ref="U78:AB78"/>
-    <mergeCell ref="U84:AB84"/>
-    <mergeCell ref="U90:AB90"/>
-    <mergeCell ref="U96:AB96"/>
-    <mergeCell ref="U102:AB102"/>
-    <mergeCell ref="M162:T162"/>
-    <mergeCell ref="M168:T168"/>
-    <mergeCell ref="M174:T174"/>
-    <mergeCell ref="M180:T180"/>
-    <mergeCell ref="U36:AB36"/>
-    <mergeCell ref="U42:AB42"/>
-    <mergeCell ref="U48:AB48"/>
-    <mergeCell ref="U54:AB54"/>
-    <mergeCell ref="U60:AB60"/>
-    <mergeCell ref="U66:AB66"/>
-    <mergeCell ref="M90:T90"/>
-    <mergeCell ref="M96:T96"/>
-    <mergeCell ref="M102:T102"/>
-    <mergeCell ref="M108:T108"/>
-    <mergeCell ref="M114:T114"/>
-    <mergeCell ref="M120:T120"/>
-    <mergeCell ref="M132:T132"/>
-    <mergeCell ref="M138:T138"/>
-    <mergeCell ref="M144:T144"/>
-    <mergeCell ref="M156:T156"/>
-    <mergeCell ref="M126:T126"/>
-    <mergeCell ref="M66:T66"/>
-    <mergeCell ref="M72:T72"/>
-    <mergeCell ref="M78:T78"/>
+    <mergeCell ref="E244:H244"/>
+    <mergeCell ref="I244:L244"/>
+    <mergeCell ref="E162:L162"/>
+    <mergeCell ref="E168:L168"/>
+    <mergeCell ref="E174:L174"/>
+    <mergeCell ref="E180:L180"/>
+    <mergeCell ref="E192:H192"/>
+    <mergeCell ref="I192:L192"/>
+    <mergeCell ref="E108:L108"/>
+    <mergeCell ref="E114:L114"/>
+    <mergeCell ref="E120:L120"/>
+    <mergeCell ref="E126:L126"/>
+    <mergeCell ref="E132:L132"/>
+    <mergeCell ref="E138:L138"/>
     <mergeCell ref="E156:L156"/>
-    <mergeCell ref="E84:L84"/>
-    <mergeCell ref="E90:L90"/>
-    <mergeCell ref="E96:L96"/>
-    <mergeCell ref="E102:L102"/>
-    <mergeCell ref="E78:L78"/>
-    <mergeCell ref="AS21:AZ21"/>
-    <mergeCell ref="AC96:AJ96"/>
-    <mergeCell ref="AC102:AJ102"/>
-    <mergeCell ref="AC108:AJ108"/>
-    <mergeCell ref="U120:AB120"/>
-    <mergeCell ref="U126:AB126"/>
-    <mergeCell ref="U132:AB132"/>
-    <mergeCell ref="U138:AB138"/>
-    <mergeCell ref="U108:AB108"/>
-    <mergeCell ref="U114:AB114"/>
-    <mergeCell ref="AK120:AR120"/>
-    <mergeCell ref="AK126:AR126"/>
-    <mergeCell ref="AK144:AR144"/>
-    <mergeCell ref="E24:L24"/>
-    <mergeCell ref="M24:T24"/>
-    <mergeCell ref="E30:L30"/>
-    <mergeCell ref="M30:T30"/>
-    <mergeCell ref="M36:T36"/>
-    <mergeCell ref="BA21:BH21"/>
-    <mergeCell ref="AC42:AJ42"/>
-    <mergeCell ref="E21:L21"/>
-    <mergeCell ref="M21:T21"/>
-    <mergeCell ref="U21:AB21"/>
-    <mergeCell ref="AC21:AJ21"/>
-    <mergeCell ref="AK21:AR21"/>
-    <mergeCell ref="M84:T84"/>
-    <mergeCell ref="E144:L144"/>
-    <mergeCell ref="BA48:BD48"/>
-    <mergeCell ref="BA66:BD66"/>
-    <mergeCell ref="BA84:BD84"/>
-    <mergeCell ref="BA102:BD102"/>
-    <mergeCell ref="BA114:BD114"/>
-    <mergeCell ref="BA120:BD120"/>
-    <mergeCell ref="M42:T42"/>
-    <mergeCell ref="M48:T48"/>
-    <mergeCell ref="M54:T54"/>
-    <mergeCell ref="M60:T60"/>
+    <mergeCell ref="E243:H243"/>
+    <mergeCell ref="I243:L243"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>